<commit_message>
functioning game ui info, some first draft weather info for cycle 1-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D95FFBEF-FA54-4D48-974D-3867B4C6197B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A3EDF2D-C3F7-4EFB-A09B-F5864FD968EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,78 @@
   </si>
   <si>
     <t>Project Sunflower</t>
+  </si>
+  <si>
+    <t>humidity</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>weatherSunny</t>
+  </si>
+  <si>
+    <t>Sunny</t>
+  </si>
+  <si>
+    <t>weatherSunnyDesc</t>
+  </si>
+  <si>
+    <t>It's always sunny.</t>
+  </si>
+  <si>
+    <t>weatherMostlyCloudy</t>
+  </si>
+  <si>
+    <t>weatherMostlyCloudyDesc</t>
+  </si>
+  <si>
+    <t>Mostly Cloudy</t>
+  </si>
+  <si>
+    <t>Clouds, clouds everywhere.</t>
+  </si>
+  <si>
+    <t>weatherPartlySunny</t>
+  </si>
+  <si>
+    <t>weatherPartlySunnyDesc</t>
+  </si>
+  <si>
+    <t>Partly Sunny</t>
+  </si>
+  <si>
+    <t>Sunny'ish.</t>
+  </si>
+  <si>
+    <t>weatherClear</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>weatherClearDesc</t>
+  </si>
+  <si>
+    <t>No clouds allowed.</t>
+  </si>
+  <si>
+    <t>weatherCloudy</t>
+  </si>
+  <si>
+    <t>weatherCloudyDesc</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
+  </si>
+  <si>
+    <t>Just clouds.</t>
   </si>
 </sst>
 </file>
@@ -376,17 +448,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -426,6 +498,102 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
initial flower growth concept
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A3EDF2D-C3F7-4EFB-A09B-F5864FD968EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{94EA8CBC-6155-49B4-983D-00AE447D5629}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Key</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Just clouds.</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>cycleStart</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>CYCLE {0}</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,97 +512,113 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gardener and weed, some more tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2E74F72E-AB31-479D-81A5-BE73CB2D0598}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A261C55-A152-4F25-90EE-A3FD9229DE71}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>He has a mallet.</t>
+  </si>
+  <si>
+    <t>unitAllyGardener</t>
+  </si>
+  <si>
+    <t>Gardener</t>
+  </si>
+  <si>
+    <t>unitAllyGardenerDesc</t>
+  </si>
+  <si>
+    <t>He gardens stuff.</t>
   </si>
 </sst>
 </file>
@@ -472,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +662,22 @@
         <v>39</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
air attacker ally and some adjustments
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1A261C55-A152-4F25-90EE-A3FD9229DE71}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E0823A2D-D45C-44B2-A84B-F35C087D619C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>He gardens stuff.</t>
+  </si>
+  <si>
+    <t>unitAllySpearman</t>
+  </si>
+  <si>
+    <t>Spear Guy</t>
+  </si>
+  <si>
+    <t>unitAllySpearmanDesc</t>
+  </si>
+  <si>
+    <t>He spears in air.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +690,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
weather forecast display, some gameplay fix/adjust/tweaks, primary level 1 plotting
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8ED6DD34-BDDE-4052-B94B-7AA630D5DD30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4BB6790B-4A5D-4C03-80FD-397EF0E06B70}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Key</t>
   </si>
@@ -296,6 +296,24 @@
   </si>
   <si>
     <t>Sahara Desert</t>
+  </si>
+  <si>
+    <t>weatherForecast</t>
+  </si>
+  <si>
+    <t>Weather Forecast</t>
+  </si>
+  <si>
+    <t>weatherLightRain</t>
+  </si>
+  <si>
+    <t>weatherLightRainDesc</t>
+  </si>
+  <si>
+    <t>Light Rain</t>
+  </si>
+  <si>
+    <t>Drip here and there.</t>
   </si>
 </sst>
 </file>
@@ -628,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,321 +762,345 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>90</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
level 1 stuff with tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4BB6790B-4A5D-4C03-80FD-397EF0E06B70}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{426092BC-3C08-44A7-BDAA-AAFB7B149FAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>Key</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>Drip here and there.</t>
+  </si>
+  <si>
+    <t>tutorialDragInstruction</t>
+  </si>
+  <si>
+    <t>Drag the card towards the playing field.</t>
   </si>
 </sst>
 </file>
@@ -646,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,6 +1110,14 @@
         <v>91</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
rest of level 1, prep level end
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{426092BC-3C08-44A7-BDAA-AAFB7B149FAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C09A5990-9837-4BAF-A1DC-BDA4BFCA4EC3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t>Key</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Drag the card towards the playing field.</t>
+  </si>
+  <si>
+    <t>cycleEnd</t>
+  </si>
+  <si>
+    <t>CYCLE COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -652,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,199 +742,199 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
         <v>57</v>
@@ -936,15 +942,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>61</v>
@@ -952,15 +958,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
         <v>64</v>
@@ -968,15 +974,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
@@ -984,15 +990,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
         <v>69</v>
@@ -1000,15 +1006,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>73</v>
@@ -1016,15 +1022,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
         <v>75</v>
@@ -1032,15 +1038,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
         <v>78</v>
@@ -1048,15 +1054,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -1064,15 +1070,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
         <v>83</v>
@@ -1080,15 +1086,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
         <v>86</v>
@@ -1096,25 +1102,33 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>98</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
level 2 stuff, level complete initial setup
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C09A5990-9837-4BAF-A1DC-BDA4BFCA4EC3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{814F1C52-39A0-4987-BDF9-86F262EA9C44}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
   <si>
     <t>Key</t>
   </si>
@@ -326,6 +326,54 @@
   </si>
   <si>
     <t>CYCLE COMPLETE</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>locationPacificNorthwest</t>
+  </si>
+  <si>
+    <t>Pacific Northwest</t>
+  </si>
+  <si>
+    <t>weatherRain</t>
+  </si>
+  <si>
+    <t>weatherRainDesc</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>Drips.</t>
+  </si>
+  <si>
+    <t>weatherOvercast</t>
+  </si>
+  <si>
+    <t>weatherOvercastDesc</t>
+  </si>
+  <si>
+    <t>Overcast</t>
+  </si>
+  <si>
+    <t>No sun.</t>
+  </si>
+  <si>
+    <t>weatherFog</t>
+  </si>
+  <si>
+    <t>weatherFogDesc</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>Condensed BS</t>
   </si>
 </sst>
 </file>
@@ -658,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,385 +798,449 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>98</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B64" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial level 4, some adjustments
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0D8B2BC4-438B-466D-9D5A-606C7E895E58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{81893D78-C4FE-4D07-9BE4-1646D0E10671}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="142">
   <si>
     <t>Key</t>
   </si>
@@ -404,6 +404,48 @@
   </si>
   <si>
     <t>danger of flying off</t>
+  </si>
+  <si>
+    <t>locationGreenland</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>weatherLightSnow</t>
+  </si>
+  <si>
+    <t>weatherLightSnowDesc</t>
+  </si>
+  <si>
+    <t>weatherSnow</t>
+  </si>
+  <si>
+    <t>weatherSnowDesc</t>
+  </si>
+  <si>
+    <t>Light Snow</t>
+  </si>
+  <si>
+    <t>a dash of snow</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>a bunch of snow</t>
+  </si>
+  <si>
+    <t>blizzard</t>
+  </si>
+  <si>
+    <t>weatherBlizzard</t>
+  </si>
+  <si>
+    <t>weatherBlizzardDesc</t>
+  </si>
+  <si>
+    <t>Blizzard</t>
   </si>
 </sst>
 </file>
@@ -736,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,265 +1094,321 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>98</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B76" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial "quiz" modal, placeholder options
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{81893D78-C4FE-4D07-9BE4-1646D0E10671}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E80B4789-BAAF-4843-90A2-B5747A8DABDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
   <si>
     <t>Key</t>
   </si>
@@ -446,6 +446,18 @@
   </si>
   <si>
     <t>Blizzard</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
   </si>
 </sst>
 </file>
@@ -778,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,569 +858,585 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>98</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more "quiz match" stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E80B4789-BAAF-4843-90A2-B5747A8DABDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6D56171-55DA-4B40-9DF3-14E36E213803}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
   <si>
     <t>Key</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>OFF</t>
+  </si>
+  <si>
+    <t>Artic</t>
   </si>
 </sst>
 </file>
@@ -792,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1352,7 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1357,7 +1360,7 @@
         <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
level complete ui art asset, target flag art asset
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0ADE7829-1441-4D18-A789-DFBEC34EA808}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10E9B270-9383-4929-B8C8-19488EBB38DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,9 +325,6 @@
     <t>cycleEnd</t>
   </si>
   <si>
-    <t>CYCLE COMPLETE</t>
-  </si>
-  <si>
     <t>victory</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>SOUND</t>
+  </si>
+  <si>
+    <t>CYCLE FINISH</t>
   </si>
 </sst>
 </file>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,50 +885,50 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
         <v>149</v>
-      </c>
-      <c r="B6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
         <v>151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
         <v>153</v>
-      </c>
-      <c r="B8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
         <v>142</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
         <v>144</v>
-      </c>
-      <c r="B10" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
         <v>147</v>
-      </c>
-      <c r="B11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,15 +952,15 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
         <v>102</v>
-      </c>
-      <c r="B15" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,130 +1101,130 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" t="s">
         <v>120</v>
-      </c>
-      <c r="B39" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" t="s">
         <v>122</v>
-      </c>
-      <c r="B40" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1469,26 +1469,26 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" t="s">
         <v>118</v>
-      </c>
-      <c r="B79" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" t="s">
         <v>104</v>
-      </c>
-      <c r="B80" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" t="s">
         <v>128</v>
-      </c>
-      <c r="B81" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
initial level select touch-up
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10E9B270-9383-4929-B8C8-19488EBB38DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3474F0EB-3833-4542-AA69-DB380E0A855F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="161">
   <si>
     <t>Key</t>
   </si>
@@ -485,6 +485,24 @@
   </si>
   <si>
     <t>CYCLE FINISH</t>
+  </si>
+  <si>
+    <t>okay</t>
+  </si>
+  <si>
+    <t>OKAY</t>
+  </si>
+  <si>
+    <t>levelMatchTitle</t>
+  </si>
+  <si>
+    <t>levelMatchDesc</t>
+  </si>
+  <si>
+    <t>MATCH CLIMATE</t>
+  </si>
+  <si>
+    <t>Find the location that matches the following climate zone and type.</t>
   </si>
 </sst>
 </file>
@@ -817,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,569 +951,593 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>98</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B85" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update level select interaction, apply ui art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3474F0EB-3833-4542-AA69-DB380E0A855F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5FF515BD-FC82-4793-B7E0-6240E686B2A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="173">
   <si>
     <t>Key</t>
   </si>
@@ -503,6 +503,42 @@
   </si>
   <si>
     <t>Find the location that matches the following climate zone and type.</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>reveal</t>
+  </si>
+  <si>
+    <t>REVEAL</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+  <si>
+    <t>levelMatchFound</t>
+  </si>
+  <si>
+    <t>Climate Match Found!</t>
+  </si>
+  <si>
+    <t>levelMatchNotFound</t>
+  </si>
+  <si>
+    <t>Climate does not match, try another location.</t>
   </si>
 </sst>
 </file>
@@ -835,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,585 +995,633 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>127</v>
+      </c>
+      <c r="B90" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>98</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B91" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more level select stuff, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4F6ECB3D-8C08-4995-9BCF-69E22FFEFD3A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A437DCA-9939-40AC-B9AF-30301C5F50E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="198">
   <si>
     <t>Key</t>
   </si>
@@ -220,9 +220,6 @@
     <t>climateTypeArid</t>
   </si>
   <si>
-    <t>Arid</t>
-  </si>
-  <si>
     <t>climateTypeAridDesc</t>
   </si>
   <si>
@@ -277,15 +274,6 @@
     <t>climateTypeRainforestDesc</t>
   </si>
   <si>
-    <t>climateTypeSubtropical</t>
-  </si>
-  <si>
-    <t>Subtropical</t>
-  </si>
-  <si>
-    <t>climateTypeSubtropicalDesc</t>
-  </si>
-  <si>
     <t>Great Plains</t>
   </si>
   <si>
@@ -502,9 +490,6 @@
     <t>MATCH CLIMATE</t>
   </si>
   <si>
-    <t>Find the location that matches the following climate zone and type.</t>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -544,10 +529,91 @@
     <t>Oceanic</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>latitude</t>
+    <t>Find the location that matches the following climate.</t>
+  </si>
+  <si>
+    <t>latitudes</t>
+  </si>
+  <si>
+    <t>Latitudes</t>
+  </si>
+  <si>
+    <t>latitudeEquator</t>
+  </si>
+  <si>
+    <t>Equator (0°)</t>
+  </si>
+  <si>
+    <t>latitudeTropicCancer</t>
+  </si>
+  <si>
+    <t>Tropic of Cancer (23°27')</t>
+  </si>
+  <si>
+    <t>latitudeTropicCapricorn</t>
+  </si>
+  <si>
+    <t>Tropic of Capricorn (23°27')</t>
+  </si>
+  <si>
+    <t>latitudeArctic</t>
+  </si>
+  <si>
+    <t>Arctic Circle (66°33')</t>
+  </si>
+  <si>
+    <t>latitudeAntarctic</t>
+  </si>
+  <si>
+    <t>Antarctic Circle (66°33')</t>
+  </si>
+  <si>
+    <t>zoneTropics</t>
+  </si>
+  <si>
+    <t>Tropics</t>
+  </si>
+  <si>
+    <t>zoneSubtropics</t>
+  </si>
+  <si>
+    <t>Subtropics</t>
+  </si>
+  <si>
+    <t>zoneTemperate</t>
+  </si>
+  <si>
+    <t>zoneFrigid</t>
+  </si>
+  <si>
+    <t>Frigid</t>
+  </si>
+  <si>
+    <t>climateZones</t>
+  </si>
+  <si>
+    <t>Climate Zones</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Desert climates are dry areas with very little rain and humidity. Not much vegitations can grow in such a place.</t>
+  </si>
+  <si>
+    <t>This is a satellite map of Earth. Here you will help us find a location that matches the climate we need to evaluate.</t>
+  </si>
+  <si>
+    <t>tutorialLevelSelect01</t>
+  </si>
+  <si>
+    <t>tutorialLevelSelect02</t>
+  </si>
+  <si>
+    <t>You can press the image of the climate to get more information.</t>
+  </si>
+  <si>
+    <t>Continental climates are found in inland areas. They generally have four seasons: spring, summer, autumn, and winter. Temperature varies from hot to cold as season changes.</t>
   </si>
 </sst>
 </file>
@@ -880,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,109 +1014,121 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="C15">
+        <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1058,7 +1136,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1066,23 +1144,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1090,7 +1168,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1098,548 +1176,640 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
         <v>175</v>
       </c>
-      <c r="B25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>163</v>
-      </c>
-      <c r="B27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>182</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>184</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>187</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B75" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>65</v>
+      </c>
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>73</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B91" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B92" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B93" t="s">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B94" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" t="s">
         <v>84</v>
       </c>
-      <c r="B84" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" t="s">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B96" t="s">
         <v>87</v>
       </c>
-      <c r="B86" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>89</v>
-      </c>
-      <c r="B87" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>90</v>
-      </c>
-      <c r="B88" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>117</v>
-      </c>
-      <c r="B89" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>103</v>
-      </c>
-      <c r="B90" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>127</v>
-      </c>
-      <c r="B91" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>98</v>
-      </c>
-      <c r="B92" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>99</v>
+      </c>
+      <c r="B98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>123</v>
+      </c>
+      <c r="B99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>194</v>
+      </c>
+      <c r="B100" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>195</v>
+      </c>
+      <c r="B101" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some more level select tweaks, added post level summary for knowledge, pretty-up post game pop-quiz
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A437DCA-9939-40AC-B9AF-30301C5F50E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{382E4799-9230-4000-8B9A-DBED4A991567}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="200">
   <si>
     <t>Key</t>
   </si>
@@ -601,19 +601,25 @@
     <t>Desert climates are dry areas with very little rain and humidity. Not much vegitations can grow in such a place.</t>
   </si>
   <si>
-    <t>This is a satellite map of Earth. Here you will help us find a location that matches the climate we need to evaluate.</t>
-  </si>
-  <si>
     <t>tutorialLevelSelect01</t>
   </si>
   <si>
     <t>tutorialLevelSelect02</t>
   </si>
   <si>
-    <t>You can press the image of the climate to get more information.</t>
-  </si>
-  <si>
     <t>Continental climates are found in inland areas. They generally have four seasons: spring, summer, autumn, and winter. Temperature varies from hot to cold as season changes.</t>
+  </si>
+  <si>
+    <t>summaryTitle</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>This is a satellite map of Earth. Here you will help us find a sutable location to land our seedling.</t>
+  </si>
+  <si>
+    <t>You can press the image of the requested climate to get more information.</t>
   </si>
 </sst>
 </file>
@@ -946,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,431 +1168,431 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B36" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B76" t="s">
         <v>57</v>
@@ -1594,15 +1600,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B78" t="s">
         <v>61</v>
@@ -1610,15 +1616,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80" t="s">
         <v>64</v>
@@ -1626,75 +1632,75 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
-      </c>
-      <c r="C81">
-        <v>0.6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B84" t="s">
-        <v>197</v>
+        <v>68</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>195</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B88" t="s">
         <v>74</v>
@@ -1702,15 +1708,15 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B90" t="s">
         <v>77</v>
@@ -1718,15 +1724,15 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B92" t="s">
         <v>141</v>
@@ -1734,15 +1740,15 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B94" t="s">
         <v>82</v>
@@ -1750,65 +1756,73 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="B100" t="s">
-        <v>193</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>194</v>
+      </c>
+      <c r="B102" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>94</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
climate and location descriptions
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2AB208CE-1C42-48F0-B154-8C7CC80D3D81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{52175E4A-8BDE-427C-A81B-7267C39A3FE4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="242">
   <si>
     <t>Key</t>
   </si>
@@ -64,9 +64,6 @@
     <t>weatherSunnyDesc</t>
   </si>
   <si>
-    <t>It's always sunny.</t>
-  </si>
-  <si>
     <t>weatherMostlyCloudy</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Mostly Cloudy</t>
   </si>
   <si>
-    <t>Clouds, clouds everywhere.</t>
-  </si>
-  <si>
     <t>weatherPartlySunny</t>
   </si>
   <si>
@@ -88,21 +82,6 @@
     <t>Partly Sunny</t>
   </si>
   <si>
-    <t>Sunny'ish.</t>
-  </si>
-  <si>
-    <t>weatherClear</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>weatherClearDesc</t>
-  </si>
-  <si>
-    <t>No clouds allowed.</t>
-  </si>
-  <si>
     <t>weatherCloudy</t>
   </si>
   <si>
@@ -112,9 +91,6 @@
     <t>Cloudy</t>
   </si>
   <si>
-    <t>Just clouds.</t>
-  </si>
-  <si>
     <t>cycle</t>
   </si>
   <si>
@@ -217,9 +193,6 @@
     <t>climateTypeMarineWestCoastDesc</t>
   </si>
   <si>
-    <t>Marine West Coast</t>
-  </si>
-  <si>
     <t>climateTypeMediterranean</t>
   </si>
   <si>
@@ -229,15 +202,6 @@
     <t>climateTypeMediterraneanDesc</t>
   </si>
   <si>
-    <t>climateTypeMonsoon</t>
-  </si>
-  <si>
-    <t>Monsoon</t>
-  </si>
-  <si>
-    <t>climateTypeMonsoonDesc</t>
-  </si>
-  <si>
     <t>climateTypePolar</t>
   </si>
   <si>
@@ -280,9 +244,6 @@
     <t>Light Rain</t>
   </si>
   <si>
-    <t>Drip here and there.</t>
-  </si>
-  <si>
     <t>tutorialDragInstruction</t>
   </si>
   <si>
@@ -313,9 +274,6 @@
     <t>Rain</t>
   </si>
   <si>
-    <t>Drips.</t>
-  </si>
-  <si>
     <t>weatherOvercast</t>
   </si>
   <si>
@@ -325,9 +283,6 @@
     <t>Overcast</t>
   </si>
   <si>
-    <t>No sun.</t>
-  </si>
-  <si>
     <t>weatherFog</t>
   </si>
   <si>
@@ -337,9 +292,6 @@
     <t>Fog</t>
   </si>
   <si>
-    <t>Condensed BS</t>
-  </si>
-  <si>
     <t>locationBritishIsles</t>
   </si>
   <si>
@@ -355,9 +307,6 @@
     <t>weatherHazeDesc</t>
   </si>
   <si>
-    <t>Bad Omen</t>
-  </si>
-  <si>
     <t>weatherSandstorm</t>
   </si>
   <si>
@@ -367,9 +316,6 @@
     <t>Sandstorm</t>
   </si>
   <si>
-    <t>danger of flying off</t>
-  </si>
-  <si>
     <t>locationGreenland</t>
   </si>
   <si>
@@ -391,18 +337,9 @@
     <t>Light Snow</t>
   </si>
   <si>
-    <t>a dash of snow</t>
-  </si>
-  <si>
     <t>Snow</t>
   </si>
   <si>
-    <t>a bunch of snow</t>
-  </si>
-  <si>
-    <t>blizzard</t>
-  </si>
-  <si>
     <t>weatherBlizzard</t>
   </si>
   <si>
@@ -424,9 +361,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>Artic</t>
-  </si>
-  <si>
     <t>close</t>
   </si>
   <si>
@@ -577,18 +511,12 @@
     <t>Desert</t>
   </si>
   <si>
-    <t>Desert climates are dry areas with very little rain and humidity. Not much vegitations can grow in such a place.</t>
-  </si>
-  <si>
     <t>tutorialLevelSelect01</t>
   </si>
   <si>
     <t>tutorialLevelSelect02</t>
   </si>
   <si>
-    <t>Continental climates are found in inland areas. They generally have four seasons: spring, summer, autumn, and winter. Temperature varies from hot to cold as season changes.</t>
-  </si>
-  <si>
     <t>summaryTitle</t>
   </si>
   <si>
@@ -667,14 +595,164 @@
     <t>Welcome to Project Bloom! We are conducting an experiment to grow these special flowers in various climates.</t>
   </si>
   <si>
-    <t>This is a satellite map of Earth. Help us find a sutable location to land our seedling based on the target climate.</t>
+    <t>This is a satellite map of Earth. Help us find a suitable location to land our seedling based on the target climate.</t>
+  </si>
+  <si>
+    <t>Desert climates are dry areas with very little rain and humidity. Not much vegetations can grow in such a place.</t>
+  </si>
+  <si>
+    <t>Sun is visible for most of the day with few scattered clouds.</t>
+  </si>
+  <si>
+    <t>Less than half the sky is covered by clouds.</t>
+  </si>
+  <si>
+    <t>Clouds cover the sky for more than 60 percent.</t>
+  </si>
+  <si>
+    <t>Clouds cover almost all of the sky.</t>
+  </si>
+  <si>
+    <t>Small amount of water accumulates from the drops of rain over the day.</t>
+  </si>
+  <si>
+    <t>Moderate amount of water accumulates from the drops of rain over the day.</t>
+  </si>
+  <si>
+    <t>Clouds cover most of the sky for more than 90%. Sun is almost invisible throughout the day.</t>
+  </si>
+  <si>
+    <t>Clouds have formed at ground level, causing low visibility.</t>
+  </si>
+  <si>
+    <t>Fine dusts cover the air, causing low visibility.</t>
+  </si>
+  <si>
+    <t>Strong wind carries a dangerous amount of sand causing massive havoc, and low visibility. Windspeed is at least 25 miles per hour (40 kilometers).</t>
+  </si>
+  <si>
+    <t>Small amount of snow accumulates over the day. Low visibility is expected.</t>
+  </si>
+  <si>
+    <t>Moderate amount of snow accumulates over the day. Low visibility is expected.</t>
+  </si>
+  <si>
+    <t>A combination of strong wind and heavy snow. Windspeed is at least 35 mph (56 kilometers), and visibility of less than 0.25 miles (400 meters).</t>
+  </si>
+  <si>
+    <t>Continental climates are found in inland areas. They generally have four seasons: spring, summer, autumn, and winter. Temperature varies from hot and cold as season changes.</t>
+  </si>
+  <si>
+    <t>Oceanic (or Maritime) climates are influenced by ocean currents and are generally located next to the sea. The temperature range is fairly narrow, with cool summers and winters.</t>
+  </si>
+  <si>
+    <t>Mediterranean climates are generally found in coastal regions, where the water is warm. The temperature is fairly warm and tropical.</t>
+  </si>
+  <si>
+    <t>Arctic</t>
+  </si>
+  <si>
+    <t>Arctic climate is defined by its long frigid winter, and short cool summer. They are at the very top and bottom of Earth where the sun barely shines.</t>
+  </si>
+  <si>
+    <t>Rainforest climate is defined by its frequent rain, and high humidity. Because of this, the area is dense with trees and vegetations.</t>
+  </si>
+  <si>
+    <t>locationOutback</t>
+  </si>
+  <si>
+    <t>locationOutbackDesc</t>
+  </si>
+  <si>
+    <t>Australian Outback</t>
+  </si>
+  <si>
+    <t>The outback is located within Australia. Its biome consists of: tropical, savanna, and desert. The most notable animal is the kangaroo.</t>
+  </si>
+  <si>
+    <t>locationSaharaDesc</t>
+  </si>
+  <si>
+    <t>locationGreatPlainsDesc</t>
+  </si>
+  <si>
+    <t>The Sahara is currently the largest hot desert in the world, located in North Africa. Its biome is predominantly desert. The most notable animal is the camel.</t>
+  </si>
+  <si>
+    <t>The Great Plains is the broad flat lands in the middle of North America. Its biome mostly consists of the prairie.  The most notable animal is the bison.</t>
+  </si>
+  <si>
+    <t>locationBritishIslesDesc</t>
+  </si>
+  <si>
+    <t>The British Isles are a group of islands located on the northwestern coast of Europe. Its biome is mostly that of a temperate forest with a wide range of woodland creatures such as the deer.</t>
+  </si>
+  <si>
+    <t>locationPacificNorthwestDesc</t>
+  </si>
+  <si>
+    <t>The Pacific Northwest is a region of North America between the Pacific Ocean and the mountain range. Its biome mostly consists of the coniferous forest (pine and evergreen trees).</t>
+  </si>
+  <si>
+    <t>locationCostaBrava</t>
+  </si>
+  <si>
+    <t>locationCostaBravaDesc</t>
+  </si>
+  <si>
+    <t>Costa Brava</t>
+  </si>
+  <si>
+    <t>Located in the northeast coastal region of Spain. Its biome consists of dry forest and scrubs.</t>
+  </si>
+  <si>
+    <t>locationGreenlandDesc</t>
+  </si>
+  <si>
+    <t>Greenland is the world’s largest island located in the North Atlantic Ocean. Its biome mostly consists of tundra. Its most notable animal is the polar bear.</t>
+  </si>
+  <si>
+    <t>locationSiberia</t>
+  </si>
+  <si>
+    <t>locationSiberiaDesc</t>
+  </si>
+  <si>
+    <t>Siberia</t>
+  </si>
+  <si>
+    <t>Siberia is a vast region north of Russia. Its biome mostly consists of snow forest (taiga). Its most notable animals are the caribou and wolves.</t>
+  </si>
+  <si>
+    <t>Brazil is a country in the upper region of South America located next to the Atlantic Ocean. Its biome mostly consists of Amazonian rainforest. Its notable animal is the jaguar.</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>locationBrazil</t>
+  </si>
+  <si>
+    <t>locationBrazilDesc</t>
+  </si>
+  <si>
+    <t>locationPuertoRico</t>
+  </si>
+  <si>
+    <t>locationPuertoRicoDesc</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Puerto Rico is a self-governed island associated with the United States located in the northeast Caribbean Sea. Its biome mostly consists of rainforest. Its notable animal is the parrot.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,6 +764,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -717,9 +802,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,103 +1138,103 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C15">
         <v>1.5</v>
@@ -1151,10 +1242,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1162,10 +1253,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1173,10 +1264,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1184,165 +1275,165 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1350,7 +1441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1358,244 +1449,328 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>28</v>
-      </c>
-      <c r="B49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
         <v>83</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>94</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B59" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="B61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B63" t="s">
+        <v>203</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>102</v>
       </c>
-      <c r="B58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>118</v>
-      </c>
-      <c r="B64" t="s">
-        <v>122</v>
+      <c r="C64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>204</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>108</v>
+      </c>
+      <c r="C66">
+        <v>1.5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>205</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>169</v>
+      </c>
+      <c r="C68">
+        <v>1.25</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>171</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="C70">
         <v>1.25</v>
@@ -1603,10 +1778,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>192</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -1614,10 +1789,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C72">
         <v>1.25</v>
@@ -1625,10 +1800,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B73" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -1636,10 +1811,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B74" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C74">
         <v>1.25</v>
@@ -1647,10 +1822,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="C75">
         <v>5</v>
@@ -1658,10 +1833,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>39</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="C76">
         <v>1.25</v>
@@ -1669,10 +1844,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -1680,21 +1855,21 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C78">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B79" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -1702,102 +1877,102 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>205</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>207</v>
-      </c>
-      <c r="C80">
-        <v>1.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>208</v>
-      </c>
-      <c r="C81">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B82" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B84" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
-        <v>57</v>
+        <v>162</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>57</v>
+        <v>192</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B88" t="s">
-        <v>184</v>
+        <v>53</v>
       </c>
       <c r="C88">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B90" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -1805,173 +1980,339 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B91" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>161</v>
+        <v>58</v>
+      </c>
+      <c r="C92">
+        <v>1.5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B93" t="s">
-        <v>65</v>
+        <v>208</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>209</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>68</v>
-      </c>
-      <c r="B95" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C95">
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="C97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="B98" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>73</v>
+        <v>213</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>217</v>
+      </c>
+      <c r="B101" t="s">
+        <v>219</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>67</v>
+      </c>
+      <c r="B102" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>216</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>90</v>
+      </c>
+      <c r="B104" t="s">
+        <v>91</v>
+      </c>
+      <c r="C104">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>220</v>
+      </c>
+      <c r="B105" t="s">
+        <v>221</v>
+      </c>
+      <c r="C105">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" t="s">
+        <v>80</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>222</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C107">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>224</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>225</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>98</v>
+      </c>
+      <c r="B110" t="s">
+        <v>99</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>228</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>230</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C112">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>231</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C113">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>236</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>237</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>238</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>239</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C117">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>185</v>
+      </c>
+      <c r="B118" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>188</v>
+      </c>
+      <c r="B119" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>163</v>
+      </c>
+      <c r="B120" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>164</v>
+      </c>
+      <c r="B121" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>74</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B122" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>76</v>
-      </c>
-      <c r="B101" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>78</v>
-      </c>
-      <c r="B102" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>79</v>
-      </c>
-      <c r="B103" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>92</v>
-      </c>
-      <c r="B105" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>116</v>
-      </c>
-      <c r="B106" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>209</v>
-      </c>
-      <c r="B107" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>212</v>
-      </c>
-      <c r="B108" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>186</v>
-      </c>
-      <c r="B109" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>187</v>
-      </c>
-      <c r="B110" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>87</v>
-      </c>
-      <c r="B111" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin and end assets, some tweaks here and there, music, initial sounds added
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{674B8FE6-7043-4319-AD25-2F3DD1337F45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AEAF36-392D-4A6B-A163-52D277BA16F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="286">
   <si>
     <t>Key</t>
   </si>
@@ -538,9 +538,6 @@
     <t>Due to the lack of water in this climate, these frogs will bring water from a nearby source. Please protect them!</t>
   </si>
   <si>
-    <t>These frogs will tend to the garden to help grow the flowers, and get rid of pesky weeds.</t>
-  </si>
-  <si>
     <t>Iron Frog</t>
   </si>
   <si>
@@ -751,9 +748,6 @@
     <t>credits</t>
   </si>
   <si>
-    <t>Written by: David Dionisio\nMusic from: Kevin Macleod\nPhotos:\nSahara (Kent Larsson), Road to the Isles (Trevor Wright), Similkameen River (Greg Shine, BLM), Costa Brava (Gordito1869), Puerto Rico (Oquendo)</t>
-  </si>
-  <si>
     <t>cycleTitle</t>
   </si>
   <si>
@@ -830,6 +824,60 @@
   </si>
   <si>
     <t>These are rare types of weather that can cause drastic change to a region. Their atmospheric condition such as wind speed and temperature are off the charts. Severe weathers are considered to be dangerous, and can put you in a perilous situation.</t>
+  </si>
+  <si>
+    <t>postGameDialog01</t>
+  </si>
+  <si>
+    <t>postGameDialog02</t>
+  </si>
+  <si>
+    <t>You have been a great help, but we need you one more time to correctly match these climates. For science!</t>
+  </si>
+  <si>
+    <t>Now that we have enough climate data of Earth, we just need to verify their category on each climate zone.</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>PROJECT SUCCESS</t>
+  </si>
+  <si>
+    <t>congrats</t>
+  </si>
+  <si>
+    <t>projectSuccess</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>creditsDesc</t>
+  </si>
+  <si>
+    <t>CREDITS</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Written by:&lt;/b&gt; David Dionisio\n&lt;b&gt;Music from:&lt;/b&gt; Kevin Macleod\n&lt;b&gt;Photos:&lt;/b&gt;\nSahara (Kent Larsson), Road to the Isles (Trevor Wright), Similkameen River (Greg Shine, BLM), Costa Brava (Gordito1869), Puerto Rico (Oquendo)</t>
+  </si>
+  <si>
+    <t>These frogs will tend to the garden to help grow the flowers, and rid them of pesky weeds.</t>
+  </si>
+  <si>
+    <t>tutorialWeatherInfo</t>
+  </si>
+  <si>
+    <t>Press any of the weather for more info!</t>
+  </si>
+  <si>
+    <t>weatherAlert</t>
+  </si>
+  <si>
+    <t>WEATHER ALERT</t>
   </si>
 </sst>
 </file>
@@ -1175,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,133 +1270,130 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16">
-        <v>1.5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1356,266 +1401,266 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>245</v>
+        <v>136</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>243</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>166</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>258</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>259</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B44" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>259</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45">
-        <v>2.5</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>284</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>285</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>193</v>
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -1623,10 +1668,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -1634,10 +1679,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -1645,10 +1690,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -1656,10 +1701,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -1667,10 +1712,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -1678,10 +1723,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -1689,10 +1734,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>197</v>
+        <v>21</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -1700,21 +1745,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -1722,10 +1767,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1733,10 +1778,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" t="s">
-        <v>199</v>
+        <v>82</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -1744,10 +1789,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1755,10 +1800,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -1766,10 +1811,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1777,43 +1822,43 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C65">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -1821,32 +1866,32 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C69">
         <v>5</v>
@@ -1854,54 +1899,54 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C70">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C71">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="C72">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C74">
         <v>1.25</v>
@@ -1909,10 +1954,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C75">
         <v>5</v>
@@ -1920,10 +1965,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C76">
         <v>1.25</v>
@@ -1931,10 +1976,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B77" t="s">
-        <v>175</v>
+        <v>281</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -1942,10 +1987,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C78">
         <v>1.25</v>
@@ -1953,10 +1998,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -1964,10 +2009,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C80">
         <v>1.25</v>
@@ -1975,10 +2020,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -1986,21 +2031,21 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C82">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -2008,80 +2053,80 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>182</v>
+      </c>
+      <c r="C84">
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>181</v>
       </c>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>183</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B88" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B90" t="s">
-        <v>162</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B91" t="s">
-        <v>192</v>
-      </c>
-      <c r="C91">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>162</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2089,21 +2134,21 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B93" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C93">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2111,10 +2156,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B95" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C95">
         <v>8</v>
@@ -2122,21 +2167,21 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B96" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="C96">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C97">
         <v>8</v>
@@ -2144,21 +2189,21 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B98" t="s">
-        <v>209</v>
+        <v>58</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>61</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>210</v>
+        <v>59</v>
+      </c>
+      <c r="B99" t="s">
+        <v>207</v>
       </c>
       <c r="C99">
         <v>8</v>
@@ -2166,10 +2211,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
-        <v>63</v>
+        <v>208</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -2177,10 +2222,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>64</v>
-      </c>
-      <c r="B101" t="s">
-        <v>211</v>
+        <v>61</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="C101">
         <v>8</v>
@@ -2188,43 +2233,43 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>212</v>
+        <v>62</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
+        <v>63</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>213</v>
+        <v>64</v>
       </c>
       <c r="B103" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C103">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>66</v>
+        <v>211</v>
       </c>
       <c r="B104" t="s">
-        <v>65</v>
+        <v>213</v>
       </c>
       <c r="C104">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B105" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C105">
         <v>10</v>
@@ -2232,20 +2277,20 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C106">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>216</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" t="s">
         <v>218</v>
       </c>
       <c r="C107">
@@ -2254,10 +2299,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B108" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C108">
         <v>2.5</v>
@@ -2265,32 +2310,32 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>220</v>
-      </c>
-      <c r="B109" t="s">
-        <v>221</v>
+        <v>215</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C109">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B110" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>222</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
+      </c>
+      <c r="B111" t="s">
+        <v>220</v>
       </c>
       <c r="C111">
         <v>12</v>
@@ -2298,109 +2343,109 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>224</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>226</v>
+        <v>79</v>
+      </c>
+      <c r="B112" t="s">
+        <v>80</v>
       </c>
       <c r="C112">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C113">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>98</v>
-      </c>
-      <c r="B114" t="s">
-        <v>99</v>
+        <v>223</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C115">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>230</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>232</v>
+        <v>98</v>
+      </c>
+      <c r="B116" t="s">
+        <v>99</v>
       </c>
       <c r="C116">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C117">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C119">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C120">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C121">
         <v>10</v>
@@ -2408,143 +2453,222 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>185</v>
-      </c>
-      <c r="B122" t="s">
-        <v>190</v>
+        <v>237</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>188</v>
-      </c>
-      <c r="B123" t="s">
-        <v>189</v>
+        <v>238</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="B124" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="B125" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="B126" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>246</v>
+        <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>247</v>
-      </c>
-      <c r="C127">
-        <v>3</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>248</v>
+        <v>74</v>
       </c>
       <c r="B128" t="s">
-        <v>251</v>
-      </c>
-      <c r="C128">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>249</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>250</v>
+        <v>282</v>
+      </c>
+      <c r="B129" t="s">
+        <v>283</v>
       </c>
       <c r="C129">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B130" t="s">
-        <v>253</v>
+        <v>245</v>
+      </c>
+      <c r="C130">
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
+        <v>249</v>
+      </c>
+      <c r="C131">
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>255</v>
-      </c>
-      <c r="B132" t="s">
-        <v>257</v>
+        <v>247</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="B133" t="s">
-        <v>263</v>
-      </c>
-      <c r="C133">
-        <v>2</v>
+        <v>251</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>264</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C134">
-        <v>10</v>
+        <v>252</v>
+      </c>
+      <c r="B134" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B135" t="s">
-        <v>268</v>
-      </c>
-      <c r="C135">
-        <v>2</v>
+        <v>255</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>260</v>
+      </c>
+      <c r="B136" t="s">
+        <v>261</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>262</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>264</v>
+      </c>
+      <c r="B138" t="s">
+        <v>266</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>265</v>
+      </c>
+      <c r="B139" t="s">
         <v>267</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>268</v>
+      </c>
+      <c r="B140" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>269</v>
       </c>
-      <c r="C136">
-        <v>10</v>
+      <c r="B141" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>275</v>
+      </c>
+      <c r="B142" t="s">
+        <v>273</v>
+      </c>
+      <c r="C142">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>274</v>
+      </c>
+      <c r="B143" t="s">
+        <v>277</v>
+      </c>
+      <c r="C143">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>272</v>
+      </c>
+      <c r="B144" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bunch of fix and tweaks, weird asset bug with sun
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AEAF36-392D-4A6B-A163-52D277BA16F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AED831B-14D3-4C3E-A5DE-C046D1C5D22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1225,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,7 +1663,7 @@
         <v>12</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
         <v>22</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>97</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
some more tweaks, text edit, initial release, marketing material
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AED831B-14D3-4C3E-A5DE-C046D1C5D22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019BB131-0A98-4DE7-90AB-1C582C261AED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,9 +430,6 @@
     <t>levelMatchFound</t>
   </si>
   <si>
-    <t>Climate Match Found!</t>
-  </si>
-  <si>
     <t>levelMatchNotFound</t>
   </si>
   <si>
@@ -442,9 +439,6 @@
     <t>Oceanic</t>
   </si>
   <si>
-    <t>Find the location that matches the following climate.</t>
-  </si>
-  <si>
     <t>latitudes</t>
   </si>
   <si>
@@ -535,21 +529,12 @@
     <t>Garden Frog</t>
   </si>
   <si>
-    <t>Due to the lack of water in this climate, these frogs will bring water from a nearby source. Please protect them!</t>
-  </si>
-  <si>
     <t>Iron Frog</t>
   </si>
   <si>
     <t>Air Frog</t>
   </si>
   <si>
-    <t>Deploy these hardy frogs to crush pesky pests and rodents from the ground.</t>
-  </si>
-  <si>
-    <t>Deploy these frogs to fight against pesky pests from the air.</t>
-  </si>
-  <si>
     <t>unitAllySunfly</t>
   </si>
   <si>
@@ -559,9 +544,6 @@
     <t>Sun Fly</t>
   </si>
   <si>
-    <t>These flies are capable of generating warmth to help flowers grow in cold weather, as well as melt frosts.</t>
-  </si>
-  <si>
     <t>unitAllyWindBlocker</t>
   </si>
   <si>
@@ -571,9 +553,6 @@
     <t>Windshield Frog</t>
   </si>
   <si>
-    <t>Deploy these frogs to protect the flowers from being blown away by dangerous winds.</t>
-  </si>
-  <si>
     <t>intro01</t>
   </si>
   <si>
@@ -589,72 +568,27 @@
     <t>We need you to help train these fine capable frogs to nurture and protect the flowers.</t>
   </si>
   <si>
-    <t>Welcome to Project Bloom! We are conducting an experiment to grow these special flowers in various climates.</t>
-  </si>
-  <si>
     <t>This is a satellite map of Earth. Help us find a suitable location to land our seedling based on the target climate.</t>
   </si>
   <si>
-    <t>Desert climates are dry areas with very little rain and humidity. Not much vegetations can grow in such a place.</t>
-  </si>
-  <si>
     <t>Sun is visible for most of the day with few scattered clouds.</t>
   </si>
   <si>
     <t>Less than half the sky is covered by clouds.</t>
   </si>
   <si>
-    <t>Clouds cover the sky for more than 60 percent.</t>
-  </si>
-  <si>
     <t>Clouds cover almost all of the sky.</t>
   </si>
   <si>
-    <t>Small amount of water accumulates from the drops of rain over the day.</t>
-  </si>
-  <si>
-    <t>Moderate amount of water accumulates from the drops of rain over the day.</t>
-  </si>
-  <si>
-    <t>Clouds cover most of the sky for more than 90%. Sun is almost invisible throughout the day.</t>
-  </si>
-  <si>
     <t>Clouds have formed at ground level, causing low visibility.</t>
   </si>
   <si>
-    <t>Fine dusts cover the air, causing low visibility.</t>
-  </si>
-  <si>
-    <t>Strong wind carries a dangerous amount of sand causing massive havoc, and low visibility. Windspeed is at least 25 miles per hour (40 kilometers).</t>
-  </si>
-  <si>
-    <t>Small amount of snow accumulates over the day. Low visibility is expected.</t>
-  </si>
-  <si>
-    <t>Moderate amount of snow accumulates over the day. Low visibility is expected.</t>
-  </si>
-  <si>
-    <t>A combination of strong wind and heavy snow. Windspeed is at least 35 mph (56 kilometers), and visibility of less than 0.25 miles (400 meters).</t>
-  </si>
-  <si>
-    <t>Continental climates are found in inland areas. They generally have four seasons: spring, summer, autumn, and winter. Temperature varies from hot and cold as season changes.</t>
-  </si>
-  <si>
-    <t>Oceanic (or Maritime) climates are influenced by ocean currents and are generally located next to the sea. The temperature range is fairly narrow, with cool summers and winters.</t>
-  </si>
-  <si>
-    <t>Mediterranean climates are generally found in coastal regions, where the water is warm. The temperature is fairly warm and tropical.</t>
-  </si>
-  <si>
     <t>Arctic</t>
   </si>
   <si>
     <t>Arctic climate is defined by its long frigid winter, and short cool summer. They are at the very top and bottom of Earth where the sun barely shines.</t>
   </si>
   <si>
-    <t>Rainforest climate is defined by its frequent rain, and high humidity. Because of this, the area is dense with trees and vegetations.</t>
-  </si>
-  <si>
     <t>locationOutback</t>
   </si>
   <si>
@@ -664,33 +598,18 @@
     <t>Australian Outback</t>
   </si>
   <si>
-    <t>The outback is located within Australia. Its biome consists of: tropical, savanna, and desert. The most notable animal is the kangaroo.</t>
-  </si>
-  <si>
     <t>locationSaharaDesc</t>
   </si>
   <si>
     <t>locationGreatPlainsDesc</t>
   </si>
   <si>
-    <t>The Sahara is currently the largest hot desert in the world, located in North Africa. Its biome is predominantly desert. The most notable animal is the camel.</t>
-  </si>
-  <si>
-    <t>The Great Plains is the broad flat lands in the middle of North America. Its biome mostly consists of the prairie.  The most notable animal is the bison.</t>
-  </si>
-  <si>
     <t>locationBritishIslesDesc</t>
   </si>
   <si>
-    <t>The British Isles are a group of islands located on the northwestern coast of Europe. Its biome is mostly that of a temperate forest with a wide range of woodland creatures such as the deer.</t>
-  </si>
-  <si>
     <t>locationPacificNorthwestDesc</t>
   </si>
   <si>
-    <t>The Pacific Northwest is a region of North America between the Pacific Ocean and the mountain range. Its biome mostly consists of the coniferous forest (pine and evergreen trees).</t>
-  </si>
-  <si>
     <t>locationCostaBrava</t>
   </si>
   <si>
@@ -700,15 +619,9 @@
     <t>Costa Brava</t>
   </si>
   <si>
-    <t>Located in the northeast coastal region of Spain. Its biome consists of dry forest and scrubs.</t>
-  </si>
-  <si>
     <t>locationGreenlandDesc</t>
   </si>
   <si>
-    <t>Greenland is the world’s largest island located in the North Atlantic Ocean. Its biome mostly consists of tundra. Its most notable animal is the polar bear.</t>
-  </si>
-  <si>
     <t>locationSiberia</t>
   </si>
   <si>
@@ -718,12 +631,6 @@
     <t>Siberia</t>
   </si>
   <si>
-    <t>Siberia is a vast region north of Russia. Its biome mostly consists of snow forest (taiga). Its most notable animals are the caribou and wolves.</t>
-  </si>
-  <si>
-    <t>Brazil is a country in the upper region of South America located next to the Atlantic Ocean. Its biome mostly consists of Amazonian rainforest. Its notable animal is the jaguar.</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -742,9 +649,6 @@
     <t>Puerto Rico</t>
   </si>
   <si>
-    <t>Puerto Rico is a self-governed island associated with the United States located in the northeast Caribbean Sea. Its biome mostly consists of rainforest. Its notable animal is the parrot.</t>
-  </si>
-  <si>
     <t>credits</t>
   </si>
   <si>
@@ -766,12 +670,6 @@
     <t>level1Summary03</t>
   </si>
   <si>
-    <t>Climate describes the pattern of weather over a long period of time at a specific region. This can be 30 years, or even over a century.</t>
-  </si>
-  <si>
-    <t>Weather describes the atmospheric condition at a specific region, and specific period of time. This is typically in hour-to-hour, day-to-day.</t>
-  </si>
-  <si>
     <t>level1Summary_ex01</t>
   </si>
   <si>
@@ -811,9 +709,6 @@
     <t>level2Summary02</t>
   </si>
   <si>
-    <t>Certain local areas can have a different pattern of weather than the main climate. This can be as small as a garden patch, or even be in a cave. As an example: a mountain or a hill can block the sunlight for most of the time, causing a cooler region.</t>
-  </si>
-  <si>
     <t>level3Summary01</t>
   </si>
   <si>
@@ -823,9 +718,6 @@
     <t>Severe Weather</t>
   </si>
   <si>
-    <t>These are rare types of weather that can cause drastic change to a region. Their atmospheric condition such as wind speed and temperature are off the charts. Severe weathers are considered to be dangerous, and can put you in a perilous situation.</t>
-  </si>
-  <si>
     <t>postGameDialog01</t>
   </si>
   <si>
@@ -878,6 +770,114 @@
   </si>
   <si>
     <t>WEATHER ALERT</t>
+  </si>
+  <si>
+    <t>Find the location that matches the climate.</t>
+  </si>
+  <si>
+    <t>Climate match found!</t>
+  </si>
+  <si>
+    <t>Clouds cover the sky for more than 60%.</t>
+  </si>
+  <si>
+    <t>A small amount of water accumulates from the rain over the day.</t>
+  </si>
+  <si>
+    <t>A moderate amount of water accumulates from the rain over the day.</t>
+  </si>
+  <si>
+    <t>Clouds cover the sky over 90%. The sun is practically invisible for the entire day.</t>
+  </si>
+  <si>
+    <t>Particles of dusts hang over the air due to the gusts of wind, causing low visibility.</t>
+  </si>
+  <si>
+    <t>Strong wind carries a dangerous amount of sand causing massive havoc, and low visibility.</t>
+  </si>
+  <si>
+    <t>A small amount of snow accumulates over the day. Low visibility is expected.</t>
+  </si>
+  <si>
+    <t>A moderate amount of snow accumulates over the day. Low visibility is expected.</t>
+  </si>
+  <si>
+    <t>A combination of strong wind, and freezing temperature. Falling large debris of ice is to be expected throughout the day.</t>
+  </si>
+  <si>
+    <t>These frogs will be gathering water from a nearby source. Please protect them as they traverse the land!</t>
+  </si>
+  <si>
+    <t>Deploy these hardy frogs to crush pesky rodents from the ground.</t>
+  </si>
+  <si>
+    <t>Deploy these frogs to fight against the pests that plague the sky.</t>
+  </si>
+  <si>
+    <t>These flies are capable of generating warmth to help flowers grow in cold weather, as well as melt ice.</t>
+  </si>
+  <si>
+    <t>Deploy these frogs to protect the flowers from being blown away by dangerous wind.</t>
+  </si>
+  <si>
+    <t>Continental climates are found in regions away from the sea. They generally have four seasons: spring, summer, autumn, and winter.</t>
+  </si>
+  <si>
+    <t>Oceanic (or Maritime) are influenced by ocean currents and are generally located next to the sea. The temperature range is fairly narrow, with cool summers and winters.</t>
+  </si>
+  <si>
+    <t>Mediterranean climates are generally found in coastal regions, where the water is warm. The temperature is mild and musty.</t>
+  </si>
+  <si>
+    <t>Rainforest climate is defined by its frequent rain, and high humidity. Because of this, these areas are dense with trees and vegetations.</t>
+  </si>
+  <si>
+    <t>The outback is located within Australia. Its biome consists of: tropical, savanna, and desert.</t>
+  </si>
+  <si>
+    <t>The Sahara is currently the largest hot desert in the world, located in North Africa. Its biome is predominantly a desert.</t>
+  </si>
+  <si>
+    <t>The Pacific Northwest is a region of North America between the Pacific Ocean and the mountain range. Its biome mostly consists of a coniferous forest (pine and evergreen trees).</t>
+  </si>
+  <si>
+    <t>The Great Plains is the broad flat lands in the middle of North America. Its biome is mostly made up of: prairie (flat grassy fields) and badlands (plateaus and canyons).</t>
+  </si>
+  <si>
+    <t>The British Isles are a group of islands located on the northwestern coast of Europe. Its biome is mostly that of a temperate forest.</t>
+  </si>
+  <si>
+    <t>Located in the northeast coastal region of Spain. Its biome consists of: dry forest and scrubs.</t>
+  </si>
+  <si>
+    <t>Puerto Rico is a self-governed island associated with the United States located in the northeast Caribbean Sea. Its biome mostly consists of a rainforest.</t>
+  </si>
+  <si>
+    <t>Brazil is a country in the upper region of South America located next to the Atlantic Ocean. Its biome mostly consists of the Amazonian rainforest.</t>
+  </si>
+  <si>
+    <t>Siberia is a vast region north of Russia. Its biome mostly consists of a snow forest (taiga).</t>
+  </si>
+  <si>
+    <t>Greenland is the world’s largest island located in the North Atlantic Ocean. Its biome mostly consists of a tundra.</t>
+  </si>
+  <si>
+    <t>Welcome to Project Bloom! We are conducting an experiment to grow some special flowers in various climates.</t>
+  </si>
+  <si>
+    <t>Weather describes the atmospheric condition at a specific region, and period of time. This is typically in hour-to-hour, day-to-day.</t>
+  </si>
+  <si>
+    <t>Climate describes the average weather over a long period of time at a specific region. This can be 30 years, or even over a century.</t>
+  </si>
+  <si>
+    <t>Certain local areas can have a different pattern of weather than the main climate. This can be as small as a garden patch, or even a cave. As an example: a mountain or a hill can block the sunlight for most of the time, causing a cooler region.</t>
+  </si>
+  <si>
+    <t>These are rare types of weather that can cause havoc across a region. Their atmospheric condition such as the wind and temperature are off the charts. Severe weathers are considered to be dangerous, and can put you in a perilous situation.</t>
+  </si>
+  <si>
+    <t>These climates are dry areas that receive little to no rain over a stretch of time. Not much vegetations can grow in these areas.</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -943,6 +943,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,23 +1271,23 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,7 +1394,7 @@
         <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1401,10 +1402,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s">
         <v>137</v>
-      </c>
-      <c r="B19" t="s">
-        <v>138</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1415,7 +1416,7 @@
         <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>251</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1423,10 +1424,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1472,10 +1473,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1499,58 +1500,58 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,23 +1564,23 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
@@ -1587,10 +1588,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1619,29 +1620,29 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="C46">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,7 +1653,7 @@
         <v>70</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,7 +1672,7 @@
         <v>13</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -1693,7 +1694,7 @@
         <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -1715,7 +1716,7 @@
         <v>15</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>194</v>
+        <v>252</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -1737,7 +1738,7 @@
         <v>21</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -1758,8 +1759,8 @@
       <c r="A57" t="s">
         <v>72</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>196</v>
+      <c r="B57" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -1780,8 +1781,8 @@
       <c r="A59" t="s">
         <v>82</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>197</v>
+      <c r="B59" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -1803,7 +1804,7 @@
         <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -1825,7 +1826,7 @@
         <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -1847,10 +1848,10 @@
         <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1869,10 +1870,10 @@
         <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1891,7 +1892,7 @@
         <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="C69">
         <v>5</v>
@@ -1913,7 +1914,7 @@
         <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -1935,7 +1936,7 @@
         <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="C73">
         <v>10</v>
@@ -1943,10 +1944,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" t="s">
         <v>167</v>
-      </c>
-      <c r="B74" t="s">
-        <v>169</v>
       </c>
       <c r="C74">
         <v>1.25</v>
@@ -1954,10 +1955,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" t="s">
-        <v>171</v>
+        <v>166</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="C75">
         <v>5</v>
@@ -1968,7 +1969,7 @@
         <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C76">
         <v>1.25</v>
@@ -1979,7 +1980,7 @@
         <v>30</v>
       </c>
       <c r="B77" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -1990,7 +1991,7 @@
         <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C78">
         <v>1.25</v>
@@ -2001,7 +2002,7 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>174</v>
+        <v>262</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -2012,7 +2013,7 @@
         <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C80">
         <v>1.25</v>
@@ -2022,8 +2023,8 @@
       <c r="A81" t="s">
         <v>32</v>
       </c>
-      <c r="B81" t="s">
-        <v>175</v>
+      <c r="B81" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -2031,10 +2032,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C82">
         <v>1.25</v>
@@ -2042,10 +2043,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>177</v>
-      </c>
-      <c r="B83" t="s">
-        <v>179</v>
+        <v>172</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -2053,10 +2054,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C84">
         <v>1.5</v>
@@ -2064,10 +2065,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>265</v>
       </c>
       <c r="C85">
         <v>5</v>
@@ -2126,7 +2127,7 @@
         <v>50</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -2136,8 +2137,8 @@
       <c r="A93" t="s">
         <v>51</v>
       </c>
-      <c r="B93" t="s">
-        <v>191</v>
+      <c r="B93" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -2158,8 +2159,8 @@
       <c r="A95" t="s">
         <v>54</v>
       </c>
-      <c r="B95" t="s">
-        <v>205</v>
+      <c r="B95" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C95">
         <v>8</v>
@@ -2170,7 +2171,7 @@
         <v>55</v>
       </c>
       <c r="B96" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2180,8 +2181,8 @@
       <c r="A97" t="s">
         <v>56</v>
       </c>
-      <c r="B97" t="s">
-        <v>206</v>
+      <c r="B97" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="C97">
         <v>8</v>
@@ -2202,8 +2203,8 @@
       <c r="A99" t="s">
         <v>59</v>
       </c>
-      <c r="B99" t="s">
-        <v>207</v>
+      <c r="B99" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="C99">
         <v>8</v>
@@ -2214,7 +2215,7 @@
         <v>60</v>
       </c>
       <c r="B100" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -2225,7 +2226,7 @@
         <v>61</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="C101">
         <v>8</v>
@@ -2247,7 +2248,7 @@
         <v>64</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>269</v>
       </c>
       <c r="C103">
         <v>8</v>
@@ -2255,10 +2256,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="B104" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="C104">
         <v>2</v>
@@ -2266,10 +2267,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="C105">
         <v>10</v>
@@ -2288,10 +2289,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B107" t="s">
-        <v>218</v>
+        <v>273</v>
       </c>
       <c r="C107">
         <v>10</v>
@@ -2310,10 +2311,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="C109">
         <v>10</v>
@@ -2332,10 +2333,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>274</v>
       </c>
       <c r="C111">
         <v>12</v>
@@ -2354,10 +2355,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="C113">
         <v>12</v>
@@ -2365,10 +2366,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="C114">
         <v>2.5</v>
@@ -2376,10 +2377,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>226</v>
+        <v>275</v>
       </c>
       <c r="C115">
         <v>8</v>
@@ -2398,10 +2399,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="C117">
         <v>10</v>
@@ -2409,10 +2410,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="C118">
         <v>1.5</v>
@@ -2420,10 +2421,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>232</v>
+        <v>278</v>
       </c>
       <c r="C119">
         <v>8</v>
@@ -2431,10 +2432,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -2442,10 +2443,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>233</v>
+        <v>277</v>
       </c>
       <c r="C121">
         <v>10</v>
@@ -2453,10 +2454,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="C122">
         <v>2</v>
@@ -2464,10 +2465,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="C123">
         <v>10</v>
@@ -2475,34 +2476,34 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B124" t="s">
-        <v>189</v>
+        <v>280</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B125" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B126" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B127" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2515,10 +2516,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="B129" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="C129">
         <v>8</v>
@@ -2526,10 +2527,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="B130" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="C130">
         <v>3</v>
@@ -2537,10 +2538,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="B131" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="C131">
         <v>10</v>
@@ -2548,10 +2549,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>248</v>
+        <v>282</v>
       </c>
       <c r="C132">
         <v>10</v>
@@ -2559,34 +2560,34 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="B133" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="B134" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
       <c r="B135" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="B136" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="C136">
         <v>2</v>
@@ -2594,10 +2595,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="C137">
         <v>10</v>
@@ -2605,10 +2606,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B138" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="C138">
         <v>2</v>
@@ -2616,10 +2617,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>265</v>
-      </c>
-      <c r="B139" t="s">
-        <v>267</v>
+        <v>230</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="C139">
         <v>10</v>
@@ -2627,37 +2628,37 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="B140" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="B141" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="C142">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="C143">
         <v>8</v>
@@ -2665,10 +2666,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="B144" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
show climate detail after entering climate match phase, update language
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019BB131-0A98-4DE7-90AB-1C582C261AED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0B367-A785-4E61-92BC-918763D06196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2137,7 @@
       <c r="A93" t="s">
         <v>51</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" t="s">
         <v>285</v>
       </c>
       <c r="C93">
@@ -2203,7 +2203,7 @@
       <c r="A99" t="s">
         <v>59</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" t="s">
         <v>268</v>
       </c>
       <c r="C99">
@@ -2225,7 +2225,7 @@
       <c r="A101" t="s">
         <v>61</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" t="s">
         <v>188</v>
       </c>
       <c r="C101">
@@ -2619,7 +2619,7 @@
       <c r="A139" t="s">
         <v>230</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" t="s">
         <v>284</v>
       </c>
       <c r="C139">

</xml_diff>

<commit_message>
added tooltip for humidity and wind speed icon for clarity
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0B367-A785-4E61-92BC-918763D06196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865C3548-7EE4-4B6C-A24E-301B4C3E68EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="288">
   <si>
     <t>Key</t>
   </si>
@@ -878,6 +878,12 @@
   </si>
   <si>
     <t>These climates are dry areas that receive little to no rain over a stretch of time. Not much vegetations can grow in these areas.</t>
+  </si>
+  <si>
+    <t>windSpeed</t>
+  </si>
+  <si>
+    <t>Wind Speed</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,471 +1626,471 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>222</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s">
-        <v>223</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
-      </c>
-      <c r="C46">
-        <v>1.5</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C48">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>184</v>
+        <v>17</v>
+      </c>
+      <c r="B51" t="s">
+        <v>19</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>252</v>
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C54">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>185</v>
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>253</v>
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>73</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>254</v>
+        <v>81</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>255</v>
+        <v>86</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>255</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>89</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>97</v>
+        <v>256</v>
       </c>
       <c r="C66">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>257</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B69" t="s">
-        <v>258</v>
+        <v>104</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B71" t="s">
-        <v>259</v>
+        <v>105</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>259</v>
       </c>
       <c r="C72">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B73" t="s">
-        <v>260</v>
+        <v>108</v>
       </c>
       <c r="C73">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>167</v>
+        <v>260</v>
       </c>
       <c r="C74">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>166</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>261</v>
+        <v>165</v>
+      </c>
+      <c r="B75" t="s">
+        <v>167</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="C76">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
+        <v>245</v>
       </c>
       <c r="C78">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>262</v>
+        <v>169</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="C80">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>32</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>263</v>
+        <v>31</v>
+      </c>
+      <c r="B81" t="s">
+        <v>170</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>171</v>
-      </c>
-      <c r="B82" t="s">
-        <v>173</v>
+        <v>32</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C82">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>172</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>264</v>
+        <v>171</v>
+      </c>
+      <c r="B83" t="s">
+        <v>173</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>174</v>
-      </c>
-      <c r="B84" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="C84">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" t="s">
-        <v>265</v>
+        <v>176</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="B86" t="s">
-        <v>42</v>
+        <v>265</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
         <v>42</v>
@@ -2092,15 +2098,15 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B89" t="s">
         <v>46</v>
@@ -2108,15 +2114,15 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B90" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" t="s">
         <v>49</v>
@@ -2124,435 +2130,432 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B92" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>285</v>
+        <v>160</v>
       </c>
       <c r="C93">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
-        <v>53</v>
+        <v>285</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>54</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>266</v>
+        <v>52</v>
+      </c>
+      <c r="B95" t="s">
+        <v>53</v>
       </c>
       <c r="C95">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>55</v>
-      </c>
-      <c r="B96" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>56</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>267</v>
+        <v>55</v>
+      </c>
+      <c r="B97" t="s">
+        <v>138</v>
       </c>
       <c r="C97">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>57</v>
-      </c>
-      <c r="B98" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="C98">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B99" t="s">
-        <v>268</v>
+        <v>58</v>
       </c>
       <c r="C99">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B100" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B101" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C101">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B103" t="s">
-        <v>269</v>
+        <v>63</v>
       </c>
       <c r="C103">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="B104" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B105" t="s">
-        <v>270</v>
+        <v>191</v>
       </c>
       <c r="C105">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B106" t="s">
-        <v>65</v>
+        <v>270</v>
       </c>
       <c r="C106">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="B107" t="s">
-        <v>273</v>
+        <v>65</v>
       </c>
       <c r="C107">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="B108" t="s">
-        <v>68</v>
+        <v>273</v>
       </c>
       <c r="C108">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>192</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>271</v>
+        <v>67</v>
+      </c>
+      <c r="B109" t="s">
+        <v>68</v>
       </c>
       <c r="C109">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>90</v>
-      </c>
-      <c r="B110" t="s">
-        <v>91</v>
+        <v>192</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C110">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B111" t="s">
-        <v>274</v>
+        <v>91</v>
       </c>
       <c r="C111">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="B112" t="s">
-        <v>80</v>
+        <v>274</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>195</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>272</v>
+        <v>79</v>
+      </c>
+      <c r="B113" t="s">
+        <v>80</v>
       </c>
       <c r="C113">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>198</v>
+        <v>272</v>
       </c>
       <c r="C114">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>275</v>
+        <v>198</v>
       </c>
       <c r="C115">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
-      </c>
-      <c r="B116" t="s">
-        <v>99</v>
+        <v>197</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>199</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>279</v>
+        <v>98</v>
+      </c>
+      <c r="B117" t="s">
+        <v>99</v>
       </c>
       <c r="C117">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>202</v>
+        <v>279</v>
       </c>
       <c r="C118">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
       <c r="C119">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="C121">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>208</v>
+        <v>277</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>276</v>
+        <v>208</v>
       </c>
       <c r="C123">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>177</v>
-      </c>
-      <c r="B124" t="s">
-        <v>280</v>
+        <v>207</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B125" t="s">
-        <v>181</v>
+        <v>280</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B126" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B127" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="B128" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="B129" t="s">
-        <v>247</v>
-      </c>
-      <c r="C129">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="B130" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="C130">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B131" t="s">
-        <v>281</v>
+        <v>213</v>
       </c>
       <c r="C131">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>215</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="B132" t="s">
+        <v>281</v>
       </c>
       <c r="C132">
         <v>10</v>
@@ -2560,115 +2563,126 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>216</v>
-      </c>
-      <c r="B133" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C133">
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B134" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B135" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B136" t="s">
-        <v>227</v>
-      </c>
-      <c r="C136">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>228</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>283</v>
+        <v>226</v>
+      </c>
+      <c r="B137" t="s">
+        <v>227</v>
       </c>
       <c r="C137">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>229</v>
-      </c>
-      <c r="B138" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B139" t="s">
-        <v>284</v>
+        <v>231</v>
       </c>
       <c r="C139">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B140" t="s">
-        <v>235</v>
+        <v>284</v>
+      </c>
+      <c r="C140">
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B141" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B142" t="s">
-        <v>237</v>
-      </c>
-      <c r="C142">
-        <v>2</v>
+        <v>234</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B143" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C143">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>238</v>
+      </c>
+      <c r="B144" t="s">
+        <v>241</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>236</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add first-time tooltip for climate zone toggles
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865C3548-7EE4-4B6C-A24E-301B4C3E68EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AE093C-27E5-4F03-AF9B-B810D239F44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="290">
   <si>
     <t>Key</t>
   </si>
@@ -884,6 +884,12 @@
   </si>
   <si>
     <t>Wind Speed</t>
+  </si>
+  <si>
+    <t>toggleClimateHint</t>
+  </si>
+  <si>
+    <t>Climate zones help determine the general temperature of climates based on the latitude. The closer you are at the equator, the more sunlight you will receive.</t>
   </si>
 </sst>
 </file>
@@ -1230,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,32 +1392,32 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="C17">
-        <v>1.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>250</v>
+        <v>126</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>250</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1419,686 +1425,689 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>251</v>
+        <v>137</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>211</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>121</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>164</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>286</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>287</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>222</v>
+        <v>286</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B47" t="s">
-        <v>249</v>
-      </c>
-      <c r="C47">
-        <v>1.5</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C49">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>184</v>
+        <v>17</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>252</v>
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C55">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>185</v>
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>253</v>
+        <v>71</v>
+      </c>
+      <c r="B58" t="s">
+        <v>73</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>254</v>
+        <v>81</v>
+      </c>
+      <c r="B60" t="s">
+        <v>83</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>255</v>
+        <v>86</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>255</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>186</v>
+        <v>89</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>256</v>
       </c>
       <c r="C67">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>257</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>258</v>
+        <v>104</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>259</v>
+        <v>105</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>259</v>
       </c>
       <c r="C73">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B74" t="s">
-        <v>260</v>
+        <v>108</v>
       </c>
       <c r="C74">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>260</v>
       </c>
       <c r="C75">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>166</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>261</v>
+        <v>165</v>
+      </c>
+      <c r="B76" t="s">
+        <v>167</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>29</v>
-      </c>
-      <c r="B77" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="C77">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B79" t="s">
-        <v>169</v>
+        <v>245</v>
       </c>
       <c r="C79">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B80" t="s">
-        <v>262</v>
+        <v>169</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
+        <v>262</v>
       </c>
       <c r="C81">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>32</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>263</v>
+        <v>31</v>
+      </c>
+      <c r="B82" t="s">
+        <v>170</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>171</v>
-      </c>
-      <c r="B83" t="s">
-        <v>173</v>
+        <v>32</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C83">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>172</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>264</v>
+        <v>171</v>
+      </c>
+      <c r="B84" t="s">
+        <v>173</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>174</v>
-      </c>
-      <c r="B85" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="C85">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>265</v>
+        <v>176</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
-        <v>42</v>
+        <v>265</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
         <v>42</v>
@@ -2106,15 +2115,15 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
         <v>46</v>
@@ -2122,15 +2131,15 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B91" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B92" t="s">
         <v>49</v>
@@ -2138,435 +2147,432 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B94" t="s">
-        <v>285</v>
+        <v>160</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B95" t="s">
-        <v>53</v>
+        <v>285</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>54</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>266</v>
+        <v>52</v>
+      </c>
+      <c r="B96" t="s">
+        <v>53</v>
       </c>
       <c r="C96">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>55</v>
-      </c>
-      <c r="B97" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>267</v>
+        <v>55</v>
+      </c>
+      <c r="B98" t="s">
+        <v>138</v>
       </c>
       <c r="C98">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>57</v>
-      </c>
-      <c r="B99" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="C99">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
-        <v>268</v>
+        <v>58</v>
       </c>
       <c r="C100">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B101" t="s">
-        <v>187</v>
+        <v>268</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B102" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C102">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B104" t="s">
-        <v>269</v>
+        <v>63</v>
       </c>
       <c r="C104">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B106" t="s">
-        <v>270</v>
+        <v>191</v>
       </c>
       <c r="C106">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B107" t="s">
-        <v>65</v>
+        <v>270</v>
       </c>
       <c r="C107">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>273</v>
+        <v>65</v>
       </c>
       <c r="C108">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>273</v>
       </c>
       <c r="C109">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>192</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>271</v>
+        <v>67</v>
+      </c>
+      <c r="B110" t="s">
+        <v>68</v>
       </c>
       <c r="C110">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>90</v>
-      </c>
-      <c r="B111" t="s">
-        <v>91</v>
+        <v>192</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C111">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B112" t="s">
-        <v>274</v>
+        <v>91</v>
       </c>
       <c r="C112">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="B113" t="s">
-        <v>80</v>
+        <v>274</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>195</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>272</v>
+        <v>79</v>
+      </c>
+      <c r="B114" t="s">
+        <v>80</v>
       </c>
       <c r="C114">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>198</v>
+        <v>272</v>
       </c>
       <c r="C115">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>275</v>
+        <v>198</v>
       </c>
       <c r="C116">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>98</v>
-      </c>
-      <c r="B117" t="s">
-        <v>99</v>
+        <v>197</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>199</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>279</v>
+        <v>98</v>
+      </c>
+      <c r="B118" t="s">
+        <v>99</v>
       </c>
       <c r="C118">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>202</v>
+        <v>279</v>
       </c>
       <c r="C119">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
       <c r="C120">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="C122">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>208</v>
+        <v>277</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>276</v>
+        <v>208</v>
       </c>
       <c r="C124">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>177</v>
-      </c>
-      <c r="B125" t="s">
-        <v>280</v>
+        <v>207</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C125">
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>280</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B127" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B128" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="B129" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
-      </c>
-      <c r="C130">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="C131">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B132" t="s">
-        <v>281</v>
+        <v>213</v>
       </c>
       <c r="C132">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>215</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="B133" t="s">
+        <v>281</v>
       </c>
       <c r="C133">
         <v>10</v>
@@ -2574,115 +2580,126 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>216</v>
-      </c>
-      <c r="B134" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B135" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B136" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B137" t="s">
-        <v>227</v>
-      </c>
-      <c r="C137">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>228</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>283</v>
+        <v>226</v>
+      </c>
+      <c r="B138" t="s">
+        <v>227</v>
       </c>
       <c r="C138">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>229</v>
-      </c>
-      <c r="B139" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B140" t="s">
-        <v>284</v>
+        <v>231</v>
       </c>
       <c r="C140">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B141" t="s">
-        <v>235</v>
+        <v>284</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B142" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
-      </c>
-      <c r="C143">
-        <v>2</v>
+        <v>234</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B144" t="s">
+        <v>237</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>238</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>241</v>
       </c>
-      <c r="C144">
+      <c r="C145">
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>236</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjustment to level 1 summary
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AE093C-27E5-4F03-AF9B-B810D239F44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D5870-7829-4E64-BFF0-BADD860C6EF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="298">
   <si>
     <t>Key</t>
   </si>
@@ -865,12 +865,6 @@
     <t>Welcome to Project Bloom! We are conducting an experiment to grow some special flowers in various climates.</t>
   </si>
   <si>
-    <t>Weather describes the atmospheric condition at a specific region, and period of time. This is typically in hour-to-hour, day-to-day.</t>
-  </si>
-  <si>
-    <t>Climate describes the average weather over a long period of time at a specific region. This can be 30 years, or even over a century.</t>
-  </si>
-  <si>
     <t>Certain local areas can have a different pattern of weather than the main climate. This can be as small as a garden patch, or even a cave. As an example: a mountain or a hill can block the sunlight for most of the time, causing a cooler region.</t>
   </si>
   <si>
@@ -890,6 +884,36 @@
   </si>
   <si>
     <t>Climate zones help determine the general temperature of climates based on the latitude. The closer you are at the equator, the more sunlight you will receive.</t>
+  </si>
+  <si>
+    <t>autumn</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Climate describes the pattern of weather in a region over a long period of time: 30 years or more.</t>
+  </si>
+  <si>
+    <t>Weather describes the atmospheric condition in a region within a period of time: hour-to-hour, day-to-day.</t>
+  </si>
+  <si>
+    <t>warmSummerColdWinter</t>
+  </si>
+  <si>
+    <t>hotYearly</t>
+  </si>
+  <si>
+    <t>Hot all year.</t>
+  </si>
+  <si>
+    <t>Warm summer, cool winter.</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D146"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,10 +1416,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1545,7 +1569,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -1553,7 +1577,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -1561,7 +1585,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -1569,7 +1593,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -1577,7 +1601,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -1585,7 +1609,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>151</v>
       </c>
@@ -1593,7 +1617,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -1601,7 +1625,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -1609,7 +1633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>156</v>
       </c>
@@ -1617,7 +1641,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -1625,7 +1649,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1633,7 +1657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1641,15 +1665,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B45" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>222</v>
       </c>
@@ -1657,7 +1681,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>225</v>
       </c>
@@ -1665,89 +1689,77 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="B48" t="s">
-        <v>249</v>
-      </c>
-      <c r="C48">
-        <v>1.5</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50">
-        <v>1.25</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C51">
-        <v>5</v>
+        <v>295</v>
+      </c>
+      <c r="B51" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>248</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>249</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>184</v>
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>70</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>252</v>
+        <v>183</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -1755,21 +1767,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -1777,10 +1789,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -1788,10 +1800,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -1799,21 +1811,21 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>82</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>254</v>
+        <v>21</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -1821,21 +1833,21 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" t="s">
-        <v>255</v>
+        <v>72</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -1843,10 +1855,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1854,10 +1866,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" t="s">
-        <v>186</v>
+        <v>82</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C65">
         <v>5</v>
@@ -1865,10 +1877,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1876,10 +1888,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -1887,21 +1899,21 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C68">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="C69">
         <v>5</v>
@@ -1909,21 +1921,21 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -1931,21 +1943,21 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B73" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -1953,43 +1965,43 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C74">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B75" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C75">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C76">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>166</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>261</v>
+        <v>103</v>
+      </c>
+      <c r="B77" t="s">
+        <v>259</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -1997,32 +2009,32 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="C78">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C80">
         <v>1.25</v>
@@ -2030,10 +2042,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>28</v>
-      </c>
-      <c r="B81" t="s">
-        <v>262</v>
+        <v>166</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -2041,10 +2053,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C82">
         <v>1.25</v>
@@ -2052,10 +2064,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>263</v>
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>245</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -2063,10 +2075,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>27</v>
       </c>
       <c r="B84" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C84">
         <v>1.25</v>
@@ -2074,10 +2086,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>172</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>264</v>
+        <v>28</v>
+      </c>
+      <c r="B85" t="s">
+        <v>262</v>
       </c>
       <c r="C85">
         <v>5</v>
@@ -2085,21 +2097,21 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C86">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>175</v>
-      </c>
-      <c r="B87" t="s">
-        <v>265</v>
+        <v>32</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C87">
         <v>5</v>
@@ -2107,102 +2119,102 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="B88" t="s">
-        <v>42</v>
+        <v>173</v>
+      </c>
+      <c r="C88">
+        <v>1.25</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>43</v>
-      </c>
-      <c r="B89" t="s">
-        <v>42</v>
+        <v>172</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="B90" t="s">
-        <v>46</v>
+        <v>176</v>
+      </c>
+      <c r="C90">
+        <v>1.5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>46</v>
+        <v>265</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B94" t="s">
-        <v>160</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B95" t="s">
-        <v>285</v>
-      </c>
-      <c r="C95">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B96" t="s">
-        <v>53</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>54</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C97">
-        <v>8</v>
+        <v>48</v>
+      </c>
+      <c r="B97" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -2210,32 +2222,32 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>56</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>267</v>
+        <v>51</v>
+      </c>
+      <c r="B99" t="s">
+        <v>283</v>
       </c>
       <c r="C99">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B100" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C100">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>59</v>
-      </c>
-      <c r="B101" t="s">
-        <v>268</v>
+        <v>54</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C101">
         <v>8</v>
@@ -2243,10 +2255,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B102" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2254,10 +2266,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>61</v>
-      </c>
-      <c r="B103" t="s">
-        <v>188</v>
+        <v>56</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="C103">
         <v>8</v>
@@ -2265,21 +2277,21 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C105">
         <v>8</v>
@@ -2287,65 +2299,65 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>189</v>
+        <v>60</v>
       </c>
       <c r="B106" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
       <c r="B107" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="C107">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B108" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C108">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="B109" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C109">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>67</v>
+        <v>189</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="C110">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>192</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>271</v>
+        <v>190</v>
+      </c>
+      <c r="B111" t="s">
+        <v>270</v>
       </c>
       <c r="C111">
         <v>10</v>
@@ -2353,54 +2365,54 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B112" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C112">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B113" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C113">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B114" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C115">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>196</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>198</v>
+        <v>90</v>
+      </c>
+      <c r="B116" t="s">
+        <v>91</v>
       </c>
       <c r="C116">
         <v>2.5</v>
@@ -2408,21 +2420,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>197</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>275</v>
+        <v>194</v>
+      </c>
+      <c r="B117" t="s">
+        <v>274</v>
       </c>
       <c r="C117">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B118" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -2430,32 +2442,32 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C119">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C120">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C121">
         <v>8</v>
@@ -2463,21 +2475,21 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>204</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>203</v>
+        <v>98</v>
+      </c>
+      <c r="B122" t="s">
+        <v>99</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C123">
         <v>10</v>
@@ -2485,200 +2497,206 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C124">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C125">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>177</v>
-      </c>
-      <c r="B126" t="s">
-        <v>280</v>
+        <v>204</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>180</v>
-      </c>
-      <c r="B127" t="s">
-        <v>181</v>
+        <v>205</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C127">
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>161</v>
-      </c>
-      <c r="B128" t="s">
-        <v>182</v>
+        <v>206</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>162</v>
-      </c>
-      <c r="B129" t="s">
-        <v>178</v>
+        <v>207</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="B130" t="s">
-        <v>75</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>246</v>
+        <v>180</v>
       </c>
       <c r="B131" t="s">
-        <v>247</v>
-      </c>
-      <c r="C131">
-        <v>8</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="B132" t="s">
-        <v>213</v>
-      </c>
-      <c r="C132">
-        <v>3</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="B133" t="s">
-        <v>281</v>
-      </c>
-      <c r="C133">
-        <v>10</v>
+        <v>178</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>215</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C134">
-        <v>10</v>
+        <v>74</v>
+      </c>
+      <c r="B134" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="B135" t="s">
-        <v>217</v>
+        <v>247</v>
+      </c>
+      <c r="C135">
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B136" t="s">
-        <v>220</v>
+        <v>213</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>219</v>
-      </c>
-      <c r="B137" t="s">
-        <v>221</v>
+        <v>214</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C137">
+        <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>226</v>
-      </c>
-      <c r="B138" t="s">
-        <v>227</v>
+        <v>215</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>228</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C139">
-        <v>10</v>
+        <v>216</v>
+      </c>
+      <c r="B139" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B140" t="s">
-        <v>231</v>
-      </c>
-      <c r="C140">
-        <v>2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B141" t="s">
-        <v>284</v>
-      </c>
-      <c r="C141">
-        <v>10</v>
+        <v>221</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B142" t="s">
-        <v>235</v>
+        <v>227</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>233</v>
-      </c>
-      <c r="B143" t="s">
-        <v>234</v>
+        <v>228</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B144" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C144">
         <v>2</v>
@@ -2686,20 +2704,58 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B145" t="s">
-        <v>241</v>
+        <v>282</v>
       </c>
       <c r="C145">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>232</v>
+      </c>
+      <c r="B146" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>233</v>
+      </c>
+      <c r="B147" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>239</v>
+      </c>
+      <c r="B148" t="s">
+        <v>237</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>238</v>
+      </c>
+      <c r="B149" t="s">
+        <v>241</v>
+      </c>
+      <c r="C149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>236</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some ui adjustments and text changes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D5870-7829-4E64-BFF0-BADD860C6EF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166FAF19-3ADC-45F2-ADFE-B08A970F9BED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,9 +883,6 @@
     <t>toggleClimateHint</t>
   </si>
   <si>
-    <t>Climate zones help determine the general temperature of climates based on the latitude. The closer you are at the equator, the more sunlight you will receive.</t>
-  </si>
-  <si>
     <t>autumn</t>
   </si>
   <si>
@@ -914,6 +911,9 @@
   </si>
   <si>
     <t>Warm summer, cool winter.</t>
+  </si>
+  <si>
+    <t>Climate zones help determine the general temperature of climates based on the latitude. Locations closer to the equator are hotter due to more direct sunlight.</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,8 +1418,8 @@
       <c r="A17" t="s">
         <v>286</v>
       </c>
-      <c r="B17" t="s">
-        <v>287</v>
+      <c r="B17" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1691,34 +1691,34 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" t="s">
         <v>288</v>
-      </c>
-      <c r="B48" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" t="s">
         <v>290</v>
-      </c>
-      <c r="B49" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
         <v>295</v>
-      </c>
-      <c r="B51" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>214</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C137">
         <v>8</v>
@@ -2639,7 +2639,7 @@
         <v>215</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C138">
         <v>10</v>

</xml_diff>

<commit_message>
updated localization with Spanish
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166FAF19-3ADC-45F2-ADFE-B08A970F9BED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944F25E-50E5-4325-AF05-7EB3EF0CF592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="435">
   <si>
     <t>Key</t>
   </si>
@@ -914,6 +915,417 @@
   </si>
   <si>
     <t>Climate zones help determine the general temperature of climates based on the latitude. Locations closer to the equator are hotter due to more direct sunlight.</t>
+  </si>
+  <si>
+    <t>Bienvenido!</t>
+  </si>
+  <si>
+    <t>PROYECTO BLOOM</t>
+  </si>
+  <si>
+    <t>CRÉDITOS</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Escrito por:&lt;/b&gt; David Dionisio\r\n&lt;b&gt;Música de:&lt;/b&gt; Kevin Macleod\r\n&lt;b&gt;Fotos:&lt;/b&gt;\r\nSahara (Kent Larsson), Camino a las Islas (Trevor Wright), Río Similkameen (Greg Shine, BLM), Costa Brava (Gordito1869), Puerto Rico (Oquendo)</t>
+  </si>
+  <si>
+    <t>LANZAMIENTO</t>
+  </si>
+  <si>
+    <t>DISCORDANCIA</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>ENCENDIDO</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>CERRAR</t>
+  </si>
+  <si>
+    <t>BIEN</t>
+  </si>
+  <si>
+    <t>REVELAR</t>
+  </si>
+  <si>
+    <t>RETROCEDER</t>
+  </si>
+  <si>
+    <t>Las zonas climáticas ayudan a determinar la temperatura general de los climas en función de la latitud. Las ubicaciones más cercanas al ecuador están más calientes debido a la luz solar más directa.</t>
+  </si>
+  <si>
+    <t>CLIMA IGUALAR</t>
+  </si>
+  <si>
+    <t>Encuentra la ubicación que coincida con el clima.</t>
+  </si>
+  <si>
+    <t>El clima no coincide, prueba con otro lugar.</t>
+  </si>
+  <si>
+    <t>¡Se encontró coincidencia climática!</t>
+  </si>
+  <si>
+    <t>Ciclo</t>
+  </si>
+  <si>
+    <t>CICLO {0}</t>
+  </si>
+  <si>
+    <t>COMENZAR</t>
+  </si>
+  <si>
+    <t>ACABADO DE CICLO</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>RESUMEN</t>
+  </si>
+  <si>
+    <t>Clima</t>
+  </si>
+  <si>
+    <t>Zona Climática</t>
+  </si>
+  <si>
+    <t>Zonas Climáticas</t>
+  </si>
+  <si>
+    <t>Ecuador (0°)</t>
+  </si>
+  <si>
+    <t>Trópico de cáncer (23°27')</t>
+  </si>
+  <si>
+    <t>Trópico de Capricornio (23°27')</t>
+  </si>
+  <si>
+    <t>Círculo Polar Ártico (66°33')</t>
+  </si>
+  <si>
+    <t>Círculo Antártico (66°33')</t>
+  </si>
+  <si>
+    <t>Zona</t>
+  </si>
+  <si>
+    <t>Trópicos</t>
+  </si>
+  <si>
+    <t>Subtrópicos</t>
+  </si>
+  <si>
+    <t>Templado</t>
+  </si>
+  <si>
+    <t>Frígido</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Humedad</t>
+  </si>
+  <si>
+    <t>Viento</t>
+  </si>
+  <si>
+    <t>Velocidad del Viento</t>
+  </si>
+  <si>
+    <t>Invierno</t>
+  </si>
+  <si>
+    <t>Verano</t>
+  </si>
+  <si>
+    <t>Otoño</t>
+  </si>
+  <si>
+    <t>Primavera</t>
+  </si>
+  <si>
+    <t>Verano cálido, invierno fresco.</t>
+  </si>
+  <si>
+    <t>Caliente todo el año.</t>
+  </si>
+  <si>
+    <t>ALERTA METEOROLÓGICA</t>
+  </si>
+  <si>
+    <t>Pronóstico Meteorológico</t>
+  </si>
+  <si>
+    <t>Soleado</t>
+  </si>
+  <si>
+    <t>El sol es visible durante la mayor parte del día con pocas nubes dispersas.</t>
+  </si>
+  <si>
+    <t>Parcialmente soleado</t>
+  </si>
+  <si>
+    <t>Menos de la mitad del cielo está cubierto de nubes.</t>
+  </si>
+  <si>
+    <t>Mayormente nublado</t>
+  </si>
+  <si>
+    <t>Las nubes cubren el cielo por más del 60%.</t>
+  </si>
+  <si>
+    <t>Nublado</t>
+  </si>
+  <si>
+    <t>Las nubes cubren casi todo el cielo.</t>
+  </si>
+  <si>
+    <t>Lluvia ligera</t>
+  </si>
+  <si>
+    <t>Una pequeña cantidad de agua se acumula de la lluvia durante el día.</t>
+  </si>
+  <si>
+    <t>Lluvia</t>
+  </si>
+  <si>
+    <t>Una cantidad moderada de agua se acumula de la lluvia durante el día.</t>
+  </si>
+  <si>
+    <t>Las nubes cubren el cielo más del 90%. El sol es prácticamente invisible durante todo el día.</t>
+  </si>
+  <si>
+    <t>Niebla</t>
+  </si>
+  <si>
+    <t>Las nubes se han formado a nivel del suelo, lo que provoca poca visibilidad.</t>
+  </si>
+  <si>
+    <t>Neblina</t>
+  </si>
+  <si>
+    <t>Las partículas de polvo cuelgan sobre el aire debido a las ráfagas de viento, lo que provoca poca visibilidad.</t>
+  </si>
+  <si>
+    <t>Tormenta de arena</t>
+  </si>
+  <si>
+    <t>El viento fuerte lleva una peligrosa cantidad de arena causando estragos masivos y baja visibilidad.</t>
+  </si>
+  <si>
+    <t>Nieve ligera</t>
+  </si>
+  <si>
+    <t>Una pequeña cantidad de nieve se acumula a lo largo del día. Se espera una baja visibilidad.</t>
+  </si>
+  <si>
+    <t>Nieve</t>
+  </si>
+  <si>
+    <t>A lo largo del día se acumula una cantidad moderada de nieve. Se espera una baja visibilidad.</t>
+  </si>
+  <si>
+    <t>Tormenta de nieve</t>
+  </si>
+  <si>
+    <t>Una combinación de viento fuerte y temperatura de congelación. Es de esperar que se caigan grandes restos de hielo durante todo el día.</t>
+  </si>
+  <si>
+    <t>Rana Recolectante</t>
+  </si>
+  <si>
+    <t>Estas ranas recolectarán agua de una fuente cercana. Por favor, protéjalos mientras atraviesan la tierra.</t>
+  </si>
+  <si>
+    <t>Rana de jardín</t>
+  </si>
+  <si>
+    <t>Estas ranas atenderán al jardín para ayudar a cultivar las flores y librarlas de malezas molestas.</t>
+  </si>
+  <si>
+    <t>Rana de hierro</t>
+  </si>
+  <si>
+    <t>Despliega estas ranas resistentes para aplastar a molestos roedores del suelo.</t>
+  </si>
+  <si>
+    <t>Rana de aire</t>
+  </si>
+  <si>
+    <t>Despliega estas ranas para luchar contra las plagas que azotan el cielo.</t>
+  </si>
+  <si>
+    <t>Mosca Solar</t>
+  </si>
+  <si>
+    <t>Estas moscas son capaces de generar calor para ayudar a que las flores crezcan en climas fríos, así como derretir hielo.</t>
+  </si>
+  <si>
+    <t>Rana del parabrisas</t>
+  </si>
+  <si>
+    <t>Despliega estas ranas para proteger las flores de la explosión del viento peligroso.</t>
+  </si>
+  <si>
+    <t>Desierto</t>
+  </si>
+  <si>
+    <t>Estos climas son áreas secas que reciben poca o ninguna lluvia durante un período de tiempo. No puede crecer mucha vegetación en estas áreas.</t>
+  </si>
+  <si>
+    <t>Los climas continentales se encuentran en regiones alejadas del mar. Generalmente tienen cuatro estaciones: primavera, verano, otoño e invierno.</t>
+  </si>
+  <si>
+    <t>Oceánico</t>
+  </si>
+  <si>
+    <t>Las corrientes oceánicas (o marítimas) están influenciadas por las corrientes oceánicas y generalmente se encuentran junto al mar. El rango de temperatura es bastante estrecho, con veranos e inviernos fríos.</t>
+  </si>
+  <si>
+    <t>Mediterráneo</t>
+  </si>
+  <si>
+    <t>Los climas mediterráneos se encuentran generalmente en regiones costeras, donde el agua es cálida. La temperatura es suave y húmeda.</t>
+  </si>
+  <si>
+    <t>Ártico</t>
+  </si>
+  <si>
+    <t>El clima ártico se define por su largo invierno helado y su corto verano fresco. Están en la parte superior e inferior de la Tierra, donde el sol apenas brilla.</t>
+  </si>
+  <si>
+    <t>Selva Tropical</t>
+  </si>
+  <si>
+    <t>El clima de la selva tropical se define por su frecuente lluvia y su alta humedad. Debido a esto, estas zonas son densas con árboles y vegetaciones.</t>
+  </si>
+  <si>
+    <t>Interior Australiano</t>
+  </si>
+  <si>
+    <t>El interior se encuentra dentro de Australia. Su bioma consiste en: tropical, sabana y desierto.</t>
+  </si>
+  <si>
+    <t>Grandes Llanuras</t>
+  </si>
+  <si>
+    <t>Las Grandes Llanuras son las amplias tierras planas en el centro de América del Norte. Su bioma se compone principalmente de: praderas (campos de hierba plana) y tierras baldías (mesetas y cañones).</t>
+  </si>
+  <si>
+    <t>Desierto del Sahara</t>
+  </si>
+  <si>
+    <t>El Sahara es actualmente el desierto caliente más grande del mundo, ubicado en el norte de África. Su bioma es predominantemente un desierto.</t>
+  </si>
+  <si>
+    <t>Islas Británicas</t>
+  </si>
+  <si>
+    <t>Las Islas Británicas son un grupo de islas situadas en la costa noroeste de Europa. Su bioma es principalmente el de un bosque templado.</t>
+  </si>
+  <si>
+    <t>Noroeste del Pacífico</t>
+  </si>
+  <si>
+    <t>El noroeste del Pacífico es una región de América del Norte entre el Océano Pacífico y la cordillera. Su bioma consiste principalmente en un bosque de coníferas (pinos y árboles perennes).</t>
+  </si>
+  <si>
+    <t>Situado en la región costera noreste de España. Su bioma consiste en: bosque seco y matorrales.</t>
+  </si>
+  <si>
+    <t>Groenlandia</t>
+  </si>
+  <si>
+    <t>Groenlandia es la isla más grande del mundo ubicada en el Océano Atlántico Norte. Su bioma consiste principalmente en una tundra.</t>
+  </si>
+  <si>
+    <t>Siberia es una vasta región al norte de Rusia. Su bioma consiste principalmente en un bosque nevado (taiga).</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Brasil es un país de la región alta de Sudamérica situado junto al Océano Atlántico. Su bioma consiste principalmente en la selva amazónica.</t>
+  </si>
+  <si>
+    <t>Puerto Rico es una isla autónoma asociada a los Estados Unidos situada en el noreste del mar Caribe. Su bioma consiste principalmente en una selva tropical.</t>
+  </si>
+  <si>
+    <t>¡Bienvenido a Project Bloom! Estamos realizando un experimento para cultivar flores especiales en varios climas.</t>
+  </si>
+  <si>
+    <t>Te necesitamos para ayudar a entrenar estas finas ranas capaces de nutrir y proteger las flores.</t>
+  </si>
+  <si>
+    <t>Ésta es un mapa satelital de Tierra. Ayúdenos a encontrar un lugar adecuado para desembarcar nuestras plántulas según el clima objetivo.</t>
+  </si>
+  <si>
+    <t>Puede presionar la imagen del clima para obtener más información.</t>
+  </si>
+  <si>
+    <t>Arrastra la carta hacia el campo de juego.</t>
+  </si>
+  <si>
+    <t>Presiona cualquier clima para obtener más información.</t>
+  </si>
+  <si>
+    <t>Clima versus Tiempo</t>
+  </si>
+  <si>
+    <t>El clima describe la condición atmosférica de una región dentro de un período de tiempo: hora a hora, día a día.</t>
+  </si>
+  <si>
+    <t>El clima describe el patrón del clima en una región durante un largo período de tiempo: 30 años o más.</t>
+  </si>
+  <si>
+    <t>Día 1</t>
+  </si>
+  <si>
+    <t>Día 2</t>
+  </si>
+  <si>
+    <t>Día 3</t>
+  </si>
+  <si>
+    <t>Microclima</t>
+  </si>
+  <si>
+    <t>Algunas zonas locales pueden tener un patrón de clima diferente al del clima principal. Esto puede ser tan pequeño como un parche de jardín o incluso una cueva. Por ejemplo: una montaña o una colina pueden bloquear la luz solar durante la mayor parte del tiempo, lo que provoca una región más fría.</t>
+  </si>
+  <si>
+    <t>Clima Severo</t>
+  </si>
+  <si>
+    <t>Estos son tipos raros de clima que pueden causar estragos en una región. Su estado atmosférico, como el viento y la temperatura, están fuera de las listas. Los climas severos se consideran peligrosos y pueden ponerlo en una situación peligrosa.</t>
+  </si>
+  <si>
+    <t>Ahora que tenemos suficientes datos climáticos de la Tierra, solo tenemos que verificar su categoría en cada zona climática.</t>
+  </si>
+  <si>
+    <t>Ha sido de gran ayuda, pero te necesitamos una vez más para que se adapte correctamente a estos climas. ¡Por ciencia!</t>
+  </si>
+  <si>
+    <t>ÉXITO DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>COMPLETAR</t>
   </si>
 </sst>
 </file>
@@ -1262,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1834,7 @@
         <v>297</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2737,7 +3149,7 @@
         <v>237</v>
       </c>
       <c r="C148">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -2748,7 +3160,7 @@
         <v>241</v>
       </c>
       <c r="C149">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -2757,6 +3169,1513 @@
       </c>
       <c r="B150" t="s">
         <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
+  <dimension ref="A1:D150"/>
+  <sheetViews>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" t="s">
+        <v>316</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B22" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>320</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>284</v>
+      </c>
+      <c r="B45" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>225</v>
+      </c>
+      <c r="B47" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>287</v>
+      </c>
+      <c r="B48" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>289</v>
+      </c>
+      <c r="B49" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>293</v>
+      </c>
+      <c r="B50" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>248</v>
+      </c>
+      <c r="B52" t="s">
+        <v>347</v>
+      </c>
+      <c r="C52">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>348</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>349</v>
+      </c>
+      <c r="C54">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" t="s">
+        <v>351</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>353</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>355</v>
+      </c>
+      <c r="C60">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>357</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" t="s">
+        <v>359</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" t="s">
+        <v>355</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
+        <v>361</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>362</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" t="s">
+        <v>363</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" t="s">
+        <v>364</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" t="s">
+        <v>365</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" t="s">
+        <v>366</v>
+      </c>
+      <c r="C72">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" t="s">
+        <v>367</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>368</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" t="s">
+        <v>369</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76" t="s">
+        <v>370</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" t="s">
+        <v>371</v>
+      </c>
+      <c r="C77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" t="s">
+        <v>372</v>
+      </c>
+      <c r="C78">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" t="s">
+        <v>373</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" t="s">
+        <v>374</v>
+      </c>
+      <c r="C80">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" t="s">
+        <v>376</v>
+      </c>
+      <c r="C82">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>377</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>27</v>
+      </c>
+      <c r="B84" t="s">
+        <v>378</v>
+      </c>
+      <c r="C84">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85" t="s">
+        <v>379</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" t="s">
+        <v>380</v>
+      </c>
+      <c r="C86">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" t="s">
+        <v>382</v>
+      </c>
+      <c r="C88">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" t="s">
+        <v>384</v>
+      </c>
+      <c r="C90">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>175</v>
+      </c>
+      <c r="B91" t="s">
+        <v>385</v>
+      </c>
+      <c r="C91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>41</v>
+      </c>
+      <c r="B92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" t="s">
+        <v>386</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>51</v>
+      </c>
+      <c r="B99" t="s">
+        <v>387</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>52</v>
+      </c>
+      <c r="B100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>55</v>
+      </c>
+      <c r="B102" t="s">
+        <v>389</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>56</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104" t="s">
+        <v>391</v>
+      </c>
+      <c r="C104">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>59</v>
+      </c>
+      <c r="B105" t="s">
+        <v>392</v>
+      </c>
+      <c r="C105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>60</v>
+      </c>
+      <c r="B106" t="s">
+        <v>393</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>61</v>
+      </c>
+      <c r="B107" t="s">
+        <v>394</v>
+      </c>
+      <c r="C107">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>62</v>
+      </c>
+      <c r="B108" t="s">
+        <v>395</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>64</v>
+      </c>
+      <c r="B109" t="s">
+        <v>396</v>
+      </c>
+      <c r="C109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>189</v>
+      </c>
+      <c r="B110" t="s">
+        <v>397</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>190</v>
+      </c>
+      <c r="B111" t="s">
+        <v>398</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>66</v>
+      </c>
+      <c r="B112" t="s">
+        <v>399</v>
+      </c>
+      <c r="C112">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>193</v>
+      </c>
+      <c r="B113" t="s">
+        <v>400</v>
+      </c>
+      <c r="C113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>67</v>
+      </c>
+      <c r="B114" t="s">
+        <v>401</v>
+      </c>
+      <c r="C114">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>90</v>
+      </c>
+      <c r="B116" t="s">
+        <v>403</v>
+      </c>
+      <c r="C116">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>194</v>
+      </c>
+      <c r="B117" t="s">
+        <v>404</v>
+      </c>
+      <c r="C117">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" t="s">
+        <v>405</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>195</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C119">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>196</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C120">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>197</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>98</v>
+      </c>
+      <c r="B122" t="s">
+        <v>408</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>199</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>200</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C124">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>201</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C125">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>204</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>205</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>206</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>207</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>177</v>
+      </c>
+      <c r="B130" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>180</v>
+      </c>
+      <c r="B131" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>161</v>
+      </c>
+      <c r="B132" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>162</v>
+      </c>
+      <c r="B133" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>74</v>
+      </c>
+      <c r="B134" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>246</v>
+      </c>
+      <c r="B135" t="s">
+        <v>419</v>
+      </c>
+      <c r="C135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>212</v>
+      </c>
+      <c r="B136" t="s">
+        <v>420</v>
+      </c>
+      <c r="C136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>214</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C137">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>215</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>216</v>
+      </c>
+      <c r="B139" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>218</v>
+      </c>
+      <c r="B140" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>219</v>
+      </c>
+      <c r="B141" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>226</v>
+      </c>
+      <c r="B142" t="s">
+        <v>426</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>228</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>229</v>
+      </c>
+      <c r="B144" t="s">
+        <v>428</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>230</v>
+      </c>
+      <c r="B145" t="s">
+        <v>429</v>
+      </c>
+      <c r="C145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>232</v>
+      </c>
+      <c r="B146" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>233</v>
+      </c>
+      <c r="B147" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>239</v>
+      </c>
+      <c r="B148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>238</v>
+      </c>
+      <c r="B149" t="s">
+        <v>433</v>
+      </c>
+      <c r="C149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>236</v>
+      </c>
+      <c r="B150" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added "new game"/"continue", improved options with sliderbar/speech toggle, ignore useless musicplaylist.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944F25E-50E5-4325-AF05-7EB3EF0CF592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46229DF4-B09E-4F73-A255-11A9C58A678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3765" yWindow="2865" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="444">
   <si>
     <t>Key</t>
   </si>
@@ -1326,6 +1326,33 @@
   </si>
   <si>
     <t>COMPLETAR</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,162 +1807,156 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>435</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>438</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18">
-        <v>1.5</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>439</v>
       </c>
       <c r="B19" t="s">
-        <v>250</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" t="s">
-        <v>137</v>
+        <v>286</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>126</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>137</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>251</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1943,246 +1964,243 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>121</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>164</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>284</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>285</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B48" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>289</v>
+        <v>222</v>
       </c>
       <c r="B49" t="s">
-        <v>290</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>293</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
-        <v>296</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B51" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="B52" t="s">
-        <v>249</v>
-      </c>
-      <c r="C52">
-        <v>1.5</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>293</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54">
-        <v>1.25</v>
+        <v>295</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>183</v>
+        <v>248</v>
+      </c>
+      <c r="B55" t="s">
+        <v>249</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -2190,984 +2208,1017 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>184</v>
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>252</v>
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C60">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>185</v>
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>16</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" t="s">
-        <v>73</v>
+        <v>15</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>253</v>
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>254</v>
+        <v>71</v>
+      </c>
+      <c r="B65" t="s">
+        <v>73</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" t="s">
-        <v>86</v>
+        <v>72</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>255</v>
+        <v>83</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" t="s">
-        <v>89</v>
+        <v>82</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>86</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>93</v>
+        <v>255</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>256</v>
+        <v>89</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>186</v>
       </c>
       <c r="C72">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>257</v>
+        <v>93</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B75" t="s">
-        <v>258</v>
+        <v>97</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B76" t="s">
-        <v>105</v>
+        <v>257</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>104</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C78">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>260</v>
+        <v>105</v>
       </c>
       <c r="C79">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
+        <v>259</v>
       </c>
       <c r="C80">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>261</v>
+        <v>106</v>
+      </c>
+      <c r="B81" t="s">
+        <v>108</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>260</v>
       </c>
       <c r="C82">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="C84">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>262</v>
+        <v>168</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>245</v>
       </c>
       <c r="C86">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>32</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>263</v>
+        <v>27</v>
+      </c>
+      <c r="B87" t="s">
+        <v>169</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>262</v>
       </c>
       <c r="C88">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>172</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>264</v>
+        <v>31</v>
+      </c>
+      <c r="B89" t="s">
+        <v>170</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>174</v>
-      </c>
-      <c r="B90" t="s">
-        <v>176</v>
+        <v>32</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C90">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>265</v>
+        <v>173</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>41</v>
-      </c>
-      <c r="B92" t="s">
-        <v>42</v>
+        <v>172</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>176</v>
+      </c>
+      <c r="C93">
+        <v>1.5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="B94" t="s">
-        <v>46</v>
+        <v>265</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B95" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B96" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B97" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B98" t="s">
-        <v>160</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
-      </c>
-      <c r="C99">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C100">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>54</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>266</v>
+        <v>50</v>
+      </c>
+      <c r="B101" t="s">
+        <v>160</v>
       </c>
       <c r="C101">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>283</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>56</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>267</v>
+        <v>52</v>
+      </c>
+      <c r="B103" t="s">
+        <v>53</v>
       </c>
       <c r="C103">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>57</v>
-      </c>
-      <c r="B104" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C104">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B105" t="s">
-        <v>268</v>
+        <v>138</v>
       </c>
       <c r="C105">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>60</v>
-      </c>
-      <c r="B106" t="s">
-        <v>187</v>
+        <v>56</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B108" t="s">
-        <v>63</v>
+        <v>268</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B109" t="s">
-        <v>269</v>
+        <v>187</v>
       </c>
       <c r="C109">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>189</v>
+        <v>61</v>
       </c>
       <c r="B110" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="B111" t="s">
-        <v>270</v>
+        <v>63</v>
       </c>
       <c r="C111">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
-        <v>65</v>
+        <v>269</v>
       </c>
       <c r="C112">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="C113">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="B114" t="s">
-        <v>68</v>
+        <v>270</v>
       </c>
       <c r="C114">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>192</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>271</v>
+        <v>66</v>
+      </c>
+      <c r="B115" t="s">
+        <v>65</v>
       </c>
       <c r="C115">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>90</v>
+        <v>193</v>
       </c>
       <c r="B116" t="s">
-        <v>91</v>
+        <v>273</v>
       </c>
       <c r="C116">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
       <c r="B117" t="s">
-        <v>274</v>
+        <v>68</v>
       </c>
       <c r="C117">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>79</v>
-      </c>
-      <c r="B118" t="s">
-        <v>80</v>
+        <v>192</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>195</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>272</v>
+        <v>90</v>
+      </c>
+      <c r="B119" t="s">
+        <v>91</v>
       </c>
       <c r="C119">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>196</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
+      </c>
+      <c r="B120" t="s">
+        <v>274</v>
       </c>
       <c r="C120">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>197</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>275</v>
+        <v>79</v>
+      </c>
+      <c r="B121" t="s">
+        <v>80</v>
       </c>
       <c r="C121">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" t="s">
-        <v>99</v>
+        <v>195</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>279</v>
+        <v>198</v>
       </c>
       <c r="C123">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>202</v>
+        <v>275</v>
       </c>
       <c r="C124">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>201</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>278</v>
+        <v>98</v>
+      </c>
+      <c r="B125" t="s">
+        <v>99</v>
       </c>
       <c r="C125">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>203</v>
+        <v>279</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>277</v>
+        <v>202</v>
       </c>
       <c r="C127">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>208</v>
+        <v>278</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>276</v>
+        <v>203</v>
       </c>
       <c r="C129">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>177</v>
-      </c>
-      <c r="B130" t="s">
-        <v>280</v>
+        <v>205</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>180</v>
-      </c>
-      <c r="B131" t="s">
-        <v>181</v>
+        <v>206</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>161</v>
-      </c>
-      <c r="B132" t="s">
-        <v>182</v>
+        <v>207</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
-        <v>178</v>
+        <v>280</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
-        <v>75</v>
+        <v>181</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
-      </c>
-      <c r="C135">
-        <v>8</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B136" t="s">
-        <v>213</v>
-      </c>
-      <c r="C136">
-        <v>3</v>
+        <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>214</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C137">
-        <v>8</v>
+        <v>74</v>
+      </c>
+      <c r="B137" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>215</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>291</v>
+        <v>246</v>
+      </c>
+      <c r="B138" t="s">
+        <v>247</v>
       </c>
       <c r="C138">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B139" t="s">
-        <v>217</v>
+        <v>213</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>218</v>
-      </c>
-      <c r="B140" t="s">
-        <v>220</v>
+        <v>214</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>219</v>
-      </c>
-      <c r="B141" t="s">
-        <v>221</v>
+        <v>215</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B142" t="s">
-        <v>227</v>
-      </c>
-      <c r="C142">
-        <v>2</v>
+        <v>217</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>228</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C143">
-        <v>10</v>
+        <v>218</v>
+      </c>
+      <c r="B143" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B144" t="s">
-        <v>231</v>
-      </c>
-      <c r="C144">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B145" t="s">
-        <v>282</v>
+        <v>227</v>
       </c>
       <c r="C145">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>232</v>
-      </c>
-      <c r="B146" t="s">
-        <v>235</v>
+        <v>228</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C146">
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B147" t="s">
-        <v>234</v>
+        <v>231</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B148" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="C148">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B149" t="s">
-        <v>241</v>
-      </c>
-      <c r="C149">
-        <v>5</v>
+        <v>235</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>233</v>
+      </c>
+      <c r="B150" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>239</v>
+      </c>
+      <c r="B151" t="s">
+        <v>237</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>238</v>
+      </c>
+      <c r="B152" t="s">
+        <v>241</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>236</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B153" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3179,10 +3230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,162 +3338,156 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>435</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>438</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
-      </c>
-      <c r="C18">
-        <v>1.5</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>439</v>
       </c>
       <c r="B19" t="s">
-        <v>315</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" t="s">
-        <v>316</v>
+        <v>286</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3450,246 +3495,243 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>326</v>
+        <v>323</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>329</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B42" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>284</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B48" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>289</v>
+        <v>222</v>
       </c>
       <c r="B49" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>293</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B51" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="B52" t="s">
-        <v>347</v>
-      </c>
-      <c r="C52">
-        <v>1.5</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>293</v>
       </c>
       <c r="B53" t="s">
-        <v>348</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="B54" t="s">
-        <v>349</v>
-      </c>
-      <c r="C54">
-        <v>1.25</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>350</v>
+        <v>248</v>
+      </c>
+      <c r="B55" t="s">
+        <v>347</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -3697,984 +3739,1017 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>352</v>
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>349</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" t="s">
-        <v>353</v>
+        <v>13</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>354</v>
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>351</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" t="s">
-        <v>355</v>
+        <v>18</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="C60">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>356</v>
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>353</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" t="s">
-        <v>357</v>
+        <v>15</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>72</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>358</v>
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>355</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" t="s">
-        <v>359</v>
+        <v>21</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>356</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>82</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>360</v>
+        <v>71</v>
+      </c>
+      <c r="B65" t="s">
+        <v>357</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" t="s">
-        <v>355</v>
+        <v>72</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>358</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" t="s">
-        <v>362</v>
+        <v>82</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>360</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C72">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B75" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B76" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C78">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C79">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C80">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>375</v>
+        <v>106</v>
+      </c>
+      <c r="B81" t="s">
+        <v>372</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C82">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84" t="s">
-        <v>378</v>
+        <v>166</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>375</v>
       </c>
       <c r="C84">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B86" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C86">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>32</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>381</v>
+        <v>27</v>
+      </c>
+      <c r="B87" t="s">
+        <v>378</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="B88" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C88">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>172</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>383</v>
+        <v>31</v>
+      </c>
+      <c r="B89" t="s">
+        <v>380</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>174</v>
-      </c>
-      <c r="B90" t="s">
-        <v>384</v>
+        <v>32</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>381</v>
       </c>
       <c r="C90">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>41</v>
-      </c>
-      <c r="B92" t="s">
-        <v>42</v>
+        <v>172</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
-        <v>42</v>
+        <v>384</v>
+      </c>
+      <c r="C93">
+        <v>1.5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="B94" t="s">
-        <v>335</v>
+        <v>385</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B95" t="s">
-        <v>335</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B96" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B97" t="s">
-        <v>49</v>
+        <v>335</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B98" t="s">
-        <v>386</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
+        <v>335</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B99" t="s">
-        <v>387</v>
-      </c>
-      <c r="C99">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C100">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>54</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>388</v>
+        <v>50</v>
+      </c>
+      <c r="B101" t="s">
+        <v>386</v>
       </c>
       <c r="C101">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B102" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>56</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>390</v>
+        <v>52</v>
+      </c>
+      <c r="B103" t="s">
+        <v>53</v>
       </c>
       <c r="C103">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>57</v>
-      </c>
-      <c r="B104" t="s">
-        <v>391</v>
+        <v>54</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>388</v>
       </c>
       <c r="C104">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B105" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C105">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>60</v>
-      </c>
-      <c r="B106" t="s">
-        <v>393</v>
+        <v>56</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>390</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B108" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B109" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C109">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>189</v>
+        <v>61</v>
       </c>
       <c r="B110" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>62</v>
       </c>
       <c r="B111" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C111">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C112">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C113">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="B114" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C114">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>192</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>402</v>
+        <v>66</v>
+      </c>
+      <c r="B115" t="s">
+        <v>399</v>
       </c>
       <c r="C115">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>90</v>
+        <v>193</v>
       </c>
       <c r="B116" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C116">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
       <c r="B117" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C117">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>79</v>
-      </c>
-      <c r="B118" t="s">
-        <v>405</v>
+        <v>192</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>402</v>
       </c>
       <c r="C118">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>195</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>406</v>
+        <v>90</v>
+      </c>
+      <c r="B119" t="s">
+        <v>403</v>
       </c>
       <c r="C119">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>196</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
+      </c>
+      <c r="B120" t="s">
+        <v>404</v>
       </c>
       <c r="C120">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>197</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>407</v>
+        <v>79</v>
+      </c>
+      <c r="B121" t="s">
+        <v>405</v>
       </c>
       <c r="C121">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" t="s">
-        <v>408</v>
+        <v>195</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>406</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>409</v>
+        <v>198</v>
       </c>
       <c r="C123">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>202</v>
+        <v>407</v>
       </c>
       <c r="C124">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>201</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>410</v>
+        <v>98</v>
+      </c>
+      <c r="B125" t="s">
+        <v>408</v>
       </c>
       <c r="C125">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>412</v>
+        <v>202</v>
       </c>
       <c r="C127">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>208</v>
+        <v>410</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C129">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>177</v>
-      </c>
-      <c r="B130" t="s">
-        <v>414</v>
+        <v>205</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>180</v>
-      </c>
-      <c r="B131" t="s">
-        <v>415</v>
+        <v>206</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>161</v>
-      </c>
-      <c r="B132" t="s">
-        <v>416</v>
+        <v>207</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="B134" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
       <c r="B135" t="s">
-        <v>419</v>
-      </c>
-      <c r="C135">
-        <v>8</v>
+        <v>416</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B136" t="s">
-        <v>420</v>
-      </c>
-      <c r="C136">
-        <v>3</v>
+        <v>417</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>214</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="C137">
-        <v>8</v>
+        <v>74</v>
+      </c>
+      <c r="B137" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>215</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>422</v>
+        <v>246</v>
+      </c>
+      <c r="B138" t="s">
+        <v>419</v>
       </c>
       <c r="C138">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B139" t="s">
-        <v>423</v>
+        <v>420</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>218</v>
-      </c>
-      <c r="B140" t="s">
-        <v>424</v>
+        <v>214</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>219</v>
-      </c>
-      <c r="B141" t="s">
-        <v>425</v>
+        <v>215</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B142" t="s">
-        <v>426</v>
-      </c>
-      <c r="C142">
-        <v>2</v>
+        <v>423</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>228</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C143">
-        <v>10</v>
+        <v>218</v>
+      </c>
+      <c r="B143" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B144" t="s">
-        <v>428</v>
-      </c>
-      <c r="C144">
-        <v>2</v>
+        <v>425</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B145" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C145">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>232</v>
-      </c>
-      <c r="B146" t="s">
-        <v>430</v>
+        <v>228</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C146">
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B147" t="s">
-        <v>431</v>
+        <v>428</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B148" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C148">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B149" t="s">
-        <v>433</v>
-      </c>
-      <c r="C149">
-        <v>5</v>
+        <v>430</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>233</v>
+      </c>
+      <c r="B150" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>239</v>
+      </c>
+      <c r="B151" t="s">
+        <v>432</v>
+      </c>
+      <c r="C151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>238</v>
+      </c>
+      <c r="B152" t="s">
+        <v>433</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>236</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B153" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more dialog in level 1 (intro to climate and weather), dialog per enemy intro.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46229DF4-B09E-4F73-A255-11A9C58A678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD9D7A4-1F0F-47FF-8F2A-D739A27F1FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3765" yWindow="2865" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="484">
   <si>
     <t>Key</t>
   </si>
@@ -725,9 +725,6 @@
     <t>postGameDialog02</t>
   </si>
   <si>
-    <t>You have been a great help, but we need you one more time to correctly match these climates. For science!</t>
-  </si>
-  <si>
     <t>Now that we have enough climate data of Earth, we just need to verify their category on each climate zone.</t>
   </si>
   <si>
@@ -1316,9 +1313,6 @@
     <t>Ahora que tenemos suficientes datos climáticos de la Tierra, solo tenemos que verificar su categoría en cada zona climática.</t>
   </si>
   <si>
-    <t>Ha sido de gran ayuda, pero te necesitamos una vez más para que se adapte correctamente a estos climas. ¡Por ciencia!</t>
-  </si>
-  <si>
     <t>ÉXITO DEL PROYECTO</t>
   </si>
   <si>
@@ -1353,6 +1347,132 @@
   </si>
   <si>
     <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>climate_title</t>
+  </si>
+  <si>
+    <t>CLIMATE</t>
+  </si>
+  <si>
+    <t>CLIMA</t>
+  </si>
+  <si>
+    <t>Ha sido de gran ayuda, pero te necesitamos una vez más para que se adapte correctamente a estos climas.</t>
+  </si>
+  <si>
+    <t>You have been a great help, but we need you one more time to correctly match these climates.</t>
+  </si>
+  <si>
+    <t>weather_title</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
+    <t>TIEMPO</t>
+  </si>
+  <si>
+    <t>intro_climate_continental_01</t>
+  </si>
+  <si>
+    <t>intro_climate_continental_02</t>
+  </si>
+  <si>
+    <t>intro_climate_continental_03</t>
+  </si>
+  <si>
+    <t>intro_climate_continental_04</t>
+  </si>
+  <si>
+    <t>Without the ocean to moderate the temperature, not much can stop the prevailing wind from being too hot, or too cold.</t>
+  </si>
+  <si>
+    <t>In this scenario, we will be growing our plants during summer. Where it is mostly sunny, with some rain here and there. A pleasant weather to be out and about, and grow our plants!</t>
+  </si>
+  <si>
+    <t>intro_weather_01</t>
+  </si>
+  <si>
+    <t>intro_weather_02</t>
+  </si>
+  <si>
+    <t>intro_weather_03</t>
+  </si>
+  <si>
+    <t>intro_weather_04</t>
+  </si>
+  <si>
+    <t>Since we will be operating during summer, take note of the weather each day.</t>
+  </si>
+  <si>
+    <t>The weather describes the atmospheric condition of a region within a period of time: how cloudy, how humid, and is it going to rain?</t>
+  </si>
+  <si>
+    <t>Remember that the climate describes the weather pattern in a region annually across 30 years or more.</t>
+  </si>
+  <si>
+    <t>So the weather we will be experiencing here over a few days will be vastly different several months later.</t>
+  </si>
+  <si>
+    <t>weed_intro_01</t>
+  </si>
+  <si>
+    <t>weed_intro_02</t>
+  </si>
+  <si>
+    <t>weed_intro_03</t>
+  </si>
+  <si>
+    <t>Watch out! It looks like weeds are starting to grow near one of our plants!</t>
+  </si>
+  <si>
+    <t>Though the weather is ideal for our plants, unfortunately so it will be for these intrusive plants.</t>
+  </si>
+  <si>
+    <t>mole_intro_01</t>
+  </si>
+  <si>
+    <t>mole_intro_02</t>
+  </si>
+  <si>
+    <t>mole_intro_03</t>
+  </si>
+  <si>
+    <t>beetle_intro_01</t>
+  </si>
+  <si>
+    <t>beetle_intro_02</t>
+  </si>
+  <si>
+    <t>beetle_intro_03</t>
+  </si>
+  <si>
+    <t>Though beetles almost eat anything, this one in particular seem to prefer eating plants.</t>
+  </si>
+  <si>
+    <t>These insects thrive in most climates, so we will be seeing more of them later.</t>
+  </si>
+  <si>
+    <t>Look out, it's a beetle!</t>
+  </si>
+  <si>
+    <t>In continental climates, the temperature varies throughout the year.</t>
+  </si>
+  <si>
+    <t>This is due to the region being within large landmasses far away from the oceans.</t>
+  </si>
+  <si>
+    <t>We must get rid of them, or else they will suck away all the nutrients that our plants need to grow!</t>
+  </si>
+  <si>
+    <t>A mole! These subterranean insectivores can be commonly found in continental climates, where the soil is ideal for making tunnels.</t>
+  </si>
+  <si>
+    <t>While moles don't have much interest in veggies, their tunneling however, can ruin a plant's roots.</t>
+  </si>
+  <si>
+    <t>Though they are essential in a healthy ecosystem, we don't want them near our plants!</t>
   </si>
 </sst>
 </file>
@@ -1699,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,15 +1874,15 @@
         <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1807,10 +1927,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,26 +1983,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>436</v>
+      </c>
+      <c r="B18" t="s">
         <v>438</v>
-      </c>
-      <c r="B18" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" t="s">
         <v>439</v>
-      </c>
-      <c r="B19" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -1904,7 +2024,7 @@
         <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1926,7 +2046,7 @@
         <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2002,249 +2122,243 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>442</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>443</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>447</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>448</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>285</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>222</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>223</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>283</v>
       </c>
       <c r="B50" t="s">
-        <v>224</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>287</v>
+        <v>222</v>
       </c>
       <c r="B51" t="s">
-        <v>288</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>289</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
       <c r="B55" t="s">
-        <v>249</v>
-      </c>
-      <c r="C55">
-        <v>1.5</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>293</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>248</v>
       </c>
       <c r="C57">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>183</v>
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>70</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -2252,10 +2366,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2263,10 +2377,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>252</v>
+        <v>184</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -2274,21 +2388,21 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C63">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>185</v>
+        <v>251</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -2296,21 +2410,21 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>253</v>
+        <v>185</v>
       </c>
       <c r="C66">
         <v>5</v>
@@ -2318,21 +2432,21 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>82</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>254</v>
+        <v>72</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C68">
         <v>5</v>
@@ -2340,10 +2454,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2351,10 +2465,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
-      </c>
-      <c r="B70" t="s">
-        <v>255</v>
+        <v>82</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="C70">
         <v>5</v>
@@ -2362,10 +2476,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2373,10 +2487,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>186</v>
+        <v>254</v>
       </c>
       <c r="C72">
         <v>5</v>
@@ -2384,10 +2498,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2395,10 +2509,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>256</v>
+        <v>186</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -2406,21 +2520,21 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C75">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C76">
         <v>5</v>
@@ -2428,21 +2542,21 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B78" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C78">
         <v>5</v>
@@ -2450,21 +2564,21 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B80" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C80">
         <v>5</v>
@@ -2472,54 +2586,54 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B81" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C81">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="C83">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>166</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>261</v>
+        <v>107</v>
+      </c>
+      <c r="B84" t="s">
+        <v>259</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C85">
         <v>1.25</v>
@@ -2527,10 +2641,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>30</v>
-      </c>
-      <c r="B86" t="s">
-        <v>245</v>
+        <v>166</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="C86">
         <v>5</v>
@@ -2538,10 +2652,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C87">
         <v>1.25</v>
@@ -2549,10 +2663,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C88">
         <v>5</v>
@@ -2560,10 +2674,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C89">
         <v>1.25</v>
@@ -2571,10 +2685,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>32</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>263</v>
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>261</v>
       </c>
       <c r="C90">
         <v>5</v>
@@ -2582,10 +2696,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C91">
         <v>1.25</v>
@@ -2593,10 +2707,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C92">
         <v>5</v>
@@ -2604,21 +2718,21 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C93">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>175</v>
-      </c>
-      <c r="B94" t="s">
-        <v>265</v>
+        <v>172</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C94">
         <v>5</v>
@@ -2626,80 +2740,80 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>176</v>
+      </c>
+      <c r="C95">
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>264</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B97" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B98" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B100" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B101" t="s">
-        <v>160</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>283</v>
-      </c>
-      <c r="C102">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -2707,21 +2821,21 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>54</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>266</v>
+        <v>51</v>
+      </c>
+      <c r="B104" t="s">
+        <v>282</v>
       </c>
       <c r="C104">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2729,10 +2843,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>56</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>267</v>
+        <v>54</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="C106">
         <v>8</v>
@@ -2740,21 +2854,21 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="C107">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B108" t="s">
-        <v>268</v>
+        <v>56</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>266</v>
       </c>
       <c r="C108">
         <v>8</v>
@@ -2762,21 +2876,21 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>58</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B110" t="s">
-        <v>188</v>
+        <v>267</v>
       </c>
       <c r="C110">
         <v>8</v>
@@ -2784,10 +2898,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B111" t="s">
-        <v>63</v>
+        <v>187</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2795,10 +2909,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>269</v>
+        <v>188</v>
       </c>
       <c r="C112">
         <v>8</v>
@@ -2806,43 +2920,43 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>189</v>
+        <v>62</v>
       </c>
       <c r="B113" t="s">
-        <v>191</v>
+        <v>63</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>190</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C114">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="B115" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="C115">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B116" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C116">
         <v>10</v>
@@ -2850,21 +2964,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B117" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C117">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>192</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>271</v>
+        <v>193</v>
+      </c>
+      <c r="B118" t="s">
+        <v>272</v>
       </c>
       <c r="C118">
         <v>10</v>
@@ -2872,10 +2986,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B119" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C119">
         <v>2.5</v>
@@ -2883,32 +2997,32 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>194</v>
-      </c>
-      <c r="B120" t="s">
-        <v>274</v>
+        <v>192</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="C120">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B121" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>195</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>272</v>
+        <v>194</v>
+      </c>
+      <c r="B122" t="s">
+        <v>273</v>
       </c>
       <c r="C122">
         <v>12</v>
@@ -2916,106 +3030,106 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>196</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>198</v>
+        <v>79</v>
+      </c>
+      <c r="B123" t="s">
+        <v>80</v>
       </c>
       <c r="C123">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C124">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>98</v>
-      </c>
-      <c r="B125" t="s">
-        <v>99</v>
+        <v>196</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="C125">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C126">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>200</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>202</v>
+        <v>98</v>
+      </c>
+      <c r="B127" t="s">
+        <v>99</v>
       </c>
       <c r="C127">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>278</v>
       </c>
       <c r="C128">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C130">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C131">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>276</v>
@@ -3026,72 +3140,72 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>177</v>
-      </c>
-      <c r="B133" t="s">
-        <v>280</v>
+        <v>206</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>180</v>
-      </c>
-      <c r="B134" t="s">
-        <v>181</v>
+        <v>207</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B135" t="s">
-        <v>182</v>
+        <v>279</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B136" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="B137" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="B138" t="s">
-        <v>247</v>
-      </c>
-      <c r="C138">
-        <v>8</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>212</v>
+        <v>74</v>
       </c>
       <c r="B139" t="s">
-        <v>213</v>
-      </c>
-      <c r="C139">
-        <v>3</v>
+        <v>75</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>214</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>292</v>
+        <v>245</v>
+      </c>
+      <c r="B140" t="s">
+        <v>246</v>
       </c>
       <c r="C140">
         <v>8</v>
@@ -3099,67 +3213,67 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>215</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>291</v>
+        <v>212</v>
+      </c>
+      <c r="B141" t="s">
+        <v>213</v>
       </c>
       <c r="C141">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>216</v>
-      </c>
-      <c r="B142" t="s">
-        <v>217</v>
+        <v>214</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C142">
+        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>218</v>
-      </c>
-      <c r="B143" t="s">
-        <v>220</v>
+        <v>215</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B144" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B145" t="s">
-        <v>227</v>
-      </c>
-      <c r="C145">
-        <v>2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>228</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C146">
-        <v>10</v>
+        <v>219</v>
+      </c>
+      <c r="B146" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B147" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C147">
         <v>2</v>
@@ -3167,10 +3281,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>230</v>
-      </c>
-      <c r="B148" t="s">
-        <v>282</v>
+        <v>228</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="C148">
         <v>10</v>
@@ -3178,62 +3292,220 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B149" t="s">
-        <v>235</v>
+        <v>231</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B150" t="s">
-        <v>234</v>
+        <v>281</v>
+      </c>
+      <c r="C150">
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B151" t="s">
-        <v>237</v>
-      </c>
-      <c r="C151">
-        <v>3</v>
+        <v>234</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B152" t="s">
-        <v>241</v>
-      </c>
-      <c r="C152">
-        <v>5</v>
+        <v>446</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>238</v>
+      </c>
+      <c r="B153" t="s">
         <v>236</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>237</v>
+      </c>
+      <c r="B154" t="s">
         <v>240</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>235</v>
+      </c>
+      <c r="B155" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>450</v>
+      </c>
+      <c r="B156" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>451</v>
+      </c>
+      <c r="B157" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>452</v>
+      </c>
+      <c r="B158" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>453</v>
+      </c>
+      <c r="B159" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>456</v>
+      </c>
+      <c r="B160" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>457</v>
+      </c>
+      <c r="B161" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>458</v>
+      </c>
+      <c r="B162" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>459</v>
+      </c>
+      <c r="B163" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>464</v>
+      </c>
+      <c r="B164" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B165" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>466</v>
+      </c>
+      <c r="B166" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>469</v>
+      </c>
+      <c r="B167" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>470</v>
+      </c>
+      <c r="B168" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>471</v>
+      </c>
+      <c r="B169" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>472</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>473</v>
+      </c>
+      <c r="B171" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>474</v>
+      </c>
+      <c r="B172" t="s">
+        <v>476</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,7 +3535,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -3277,7 +3549,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,15 +3557,15 @@
         <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,7 +3573,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3309,7 +3581,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3317,7 +3589,7 @@
         <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3325,7 +3597,7 @@
         <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3333,15 +3605,15 @@
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>433</v>
+      </c>
+      <c r="B11" t="s">
         <v>435</v>
-      </c>
-      <c r="B11" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3349,7 +3621,7 @@
         <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3357,7 +3629,7 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3365,7 +3637,7 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3373,7 +3645,7 @@
         <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3381,7 +3653,7 @@
         <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3389,31 +3661,31 @@
         <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B19" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -3424,7 +3696,7 @@
         <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C21">
         <v>1.5</v>
@@ -3435,7 +3707,7 @@
         <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -3446,7 +3718,7 @@
         <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -3457,7 +3729,7 @@
         <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3468,7 +3740,7 @@
         <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3479,7 +3751,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3487,7 +3759,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3498,7 +3770,7 @@
         <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -3509,7 +3781,7 @@
         <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3517,7 +3789,7 @@
         <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3528,254 +3800,248 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>442</v>
       </c>
       <c r="B32" t="s">
-        <v>325</v>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>447</v>
       </c>
       <c r="B35" t="s">
-        <v>327</v>
+        <v>449</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>328</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B42" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>222</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>283</v>
       </c>
       <c r="B50" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>287</v>
+        <v>222</v>
       </c>
       <c r="B51" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>289</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
       <c r="B55" t="s">
-        <v>347</v>
-      </c>
-      <c r="C55">
-        <v>1.5</v>
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>293</v>
       </c>
       <c r="B56" t="s">
-        <v>348</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C57">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>350</v>
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>347</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -3783,10 +4049,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -3794,10 +4060,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -3805,21 +4071,21 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C63">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -3827,21 +4093,21 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C66">
         <v>5</v>
@@ -3849,21 +4115,21 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>82</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>360</v>
+        <v>72</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="C68">
         <v>5</v>
@@ -3871,10 +4137,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3882,10 +4148,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
-      </c>
-      <c r="B70" t="s">
-        <v>361</v>
+        <v>82</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>359</v>
       </c>
       <c r="C70">
         <v>5</v>
@@ -3893,10 +4159,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3904,10 +4170,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C72">
         <v>5</v>
@@ -3915,10 +4181,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3926,10 +4192,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -3937,21 +4203,21 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C75">
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B76" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C76">
         <v>5</v>
@@ -3959,21 +4225,21 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B78" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C78">
         <v>5</v>
@@ -3981,21 +4247,21 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B79" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B80" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C80">
         <v>5</v>
@@ -4003,54 +4269,54 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B81" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C81">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C83">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>166</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>375</v>
+        <v>107</v>
+      </c>
+      <c r="B84" t="s">
+        <v>372</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C85">
         <v>1.25</v>
@@ -4058,10 +4324,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>30</v>
-      </c>
-      <c r="B86" t="s">
-        <v>377</v>
+        <v>166</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>374</v>
       </c>
       <c r="C86">
         <v>5</v>
@@ -4069,10 +4335,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C87">
         <v>1.25</v>
@@ -4080,10 +4346,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C88">
         <v>5</v>
@@ -4091,10 +4357,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C89">
         <v>1.25</v>
@@ -4102,10 +4368,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>32</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>381</v>
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>378</v>
       </c>
       <c r="C90">
         <v>5</v>
@@ -4113,10 +4379,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C91">
         <v>1.25</v>
@@ -4124,10 +4390,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C92">
         <v>5</v>
@@ -4135,21 +4401,21 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B93" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C93">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>175</v>
-      </c>
-      <c r="B94" t="s">
-        <v>385</v>
+        <v>172</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>382</v>
       </c>
       <c r="C94">
         <v>5</v>
@@ -4157,80 +4423,80 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>383</v>
+      </c>
+      <c r="C95">
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>384</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B97" t="s">
-        <v>335</v>
+        <v>42</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B98" t="s">
-        <v>335</v>
+        <v>42</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>334</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B100" t="s">
-        <v>49</v>
+        <v>334</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B101" t="s">
-        <v>386</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>387</v>
-      </c>
-      <c r="C102">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>385</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -4238,21 +4504,21 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>54</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>388</v>
+        <v>51</v>
+      </c>
+      <c r="B104" t="s">
+        <v>386</v>
       </c>
       <c r="C104">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B105" t="s">
-        <v>389</v>
+        <v>53</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -4260,10 +4526,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>56</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>390</v>
+        <v>54</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>387</v>
       </c>
       <c r="C106">
         <v>8</v>
@@ -4271,21 +4537,21 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B107" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C107">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>59</v>
-      </c>
-      <c r="B108" t="s">
-        <v>392</v>
+        <v>56</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C108">
         <v>8</v>
@@ -4293,21 +4559,21 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B110" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C110">
         <v>8</v>
@@ -4315,10 +4581,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B111" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -4326,10 +4592,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C112">
         <v>8</v>
@@ -4337,43 +4603,43 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>189</v>
+        <v>62</v>
       </c>
       <c r="B113" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>190</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C114">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="B115" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C115">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B116" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C116">
         <v>10</v>
@@ -4381,21 +4647,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B117" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C117">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>192</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>402</v>
+        <v>193</v>
+      </c>
+      <c r="B118" t="s">
+        <v>399</v>
       </c>
       <c r="C118">
         <v>10</v>
@@ -4403,10 +4669,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B119" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C119">
         <v>2.5</v>
@@ -4414,32 +4680,32 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>194</v>
-      </c>
-      <c r="B120" t="s">
-        <v>404</v>
+        <v>192</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C120">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B121" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>195</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>406</v>
+        <v>194</v>
+      </c>
+      <c r="B122" t="s">
+        <v>403</v>
       </c>
       <c r="C122">
         <v>12</v>
@@ -4447,109 +4713,109 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>196</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>198</v>
+        <v>79</v>
+      </c>
+      <c r="B123" t="s">
+        <v>404</v>
       </c>
       <c r="C123">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C124">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>98</v>
-      </c>
-      <c r="B125" t="s">
-        <v>408</v>
+        <v>196</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="C125">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C126">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>200</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>202</v>
+        <v>98</v>
+      </c>
+      <c r="B127" t="s">
+        <v>407</v>
       </c>
       <c r="C127">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C128">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>411</v>
+        <v>202</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C130">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>208</v>
+        <v>410</v>
       </c>
       <c r="C131">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C132">
         <v>10</v>
@@ -4557,72 +4823,72 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>177</v>
-      </c>
-      <c r="B133" t="s">
-        <v>414</v>
+        <v>206</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>180</v>
-      </c>
-      <c r="B134" t="s">
-        <v>415</v>
+        <v>207</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B135" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B136" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="B137" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="B138" t="s">
-        <v>419</v>
-      </c>
-      <c r="C138">
-        <v>8</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>212</v>
+        <v>74</v>
       </c>
       <c r="B139" t="s">
-        <v>420</v>
-      </c>
-      <c r="C139">
-        <v>3</v>
+        <v>417</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>214</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>421</v>
+        <v>245</v>
+      </c>
+      <c r="B140" t="s">
+        <v>418</v>
       </c>
       <c r="C140">
         <v>8</v>
@@ -4630,67 +4896,67 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>215</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>422</v>
+        <v>212</v>
+      </c>
+      <c r="B141" t="s">
+        <v>419</v>
       </c>
       <c r="C141">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>216</v>
-      </c>
-      <c r="B142" t="s">
-        <v>423</v>
+        <v>214</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C142">
+        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>218</v>
-      </c>
-      <c r="B143" t="s">
-        <v>424</v>
+        <v>215</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B144" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B145" t="s">
-        <v>426</v>
-      </c>
-      <c r="C145">
-        <v>2</v>
+        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>228</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C146">
-        <v>10</v>
+        <v>219</v>
+      </c>
+      <c r="B146" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B147" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C147">
         <v>2</v>
@@ -4698,10 +4964,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>230</v>
-      </c>
-      <c r="B148" t="s">
-        <v>429</v>
+        <v>228</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>426</v>
       </c>
       <c r="C148">
         <v>10</v>
@@ -4709,48 +4975,155 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B149" t="s">
-        <v>430</v>
+        <v>427</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B150" t="s">
-        <v>431</v>
+        <v>428</v>
+      </c>
+      <c r="C150">
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B151" t="s">
-        <v>432</v>
-      </c>
-      <c r="C151">
-        <v>3</v>
+        <v>429</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B152" t="s">
-        <v>433</v>
-      </c>
-      <c r="C152">
-        <v>5</v>
+        <v>445</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B153" t="s">
-        <v>434</v>
+        <v>430</v>
+      </c>
+      <c r="C153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>237</v>
+      </c>
+      <c r="B154" t="s">
+        <v>431</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>235</v>
+      </c>
+      <c r="B155" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added intro dialogs to level 2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD9D7A4-1F0F-47FF-8F2A-D739A27F1FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38126D0-1DEE-4445-B985-5DB131DED054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2865" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4455" yWindow="2355" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="511">
   <si>
     <t>Key</t>
   </si>
@@ -1448,9 +1448,6 @@
     <t>beetle_intro_03</t>
   </si>
   <si>
-    <t>Though beetles almost eat anything, this one in particular seem to prefer eating plants.</t>
-  </si>
-  <si>
     <t>These insects thrive in most climates, so we will be seeing more of them later.</t>
   </si>
   <si>
@@ -1473,6 +1470,90 @@
   </si>
   <si>
     <t>Though they are essential in a healthy ecosystem, we don't want them near our plants!</t>
+  </si>
+  <si>
+    <t>coolRainyAnnually</t>
+  </si>
+  <si>
+    <t>Cool and rainy most of the year.</t>
+  </si>
+  <si>
+    <t>microclimate_title</t>
+  </si>
+  <si>
+    <t>MICROCLIMATE</t>
+  </si>
+  <si>
+    <t>MICROCLIMA</t>
+  </si>
+  <si>
+    <t>Though beetles almost eat anything, this one in particular seems to prefer eating plants.</t>
+  </si>
+  <si>
+    <t>intro_climate_oceanic_01</t>
+  </si>
+  <si>
+    <t>intro_climate_oceanic_02</t>
+  </si>
+  <si>
+    <t>intro_climate_oceanic_03</t>
+  </si>
+  <si>
+    <t>intro_climate_oceanic_04</t>
+  </si>
+  <si>
+    <t>intro_microclimate_01</t>
+  </si>
+  <si>
+    <t>intro_microclimate_02</t>
+  </si>
+  <si>
+    <t>intro_microclimate_03</t>
+  </si>
+  <si>
+    <t>mushroom_intro_01</t>
+  </si>
+  <si>
+    <t>mushroom_intro_02</t>
+  </si>
+  <si>
+    <t>mushroom_intro_03</t>
+  </si>
+  <si>
+    <t>mushroom_intro_04</t>
+  </si>
+  <si>
+    <t>Ah, the oceanic climate! Where it’s nice and cool throughout the year!</t>
+  </si>
+  <si>
+    <t>This is due to the region being close to the ocean that regulates the temperature.</t>
+  </si>
+  <si>
+    <t>However, the winds carrying the nice ocean breeze can cause a lot of days to be dull and dreary.</t>
+  </si>
+  <si>
+    <t>Nevertheless, this moody atmosphere is a perfect place to grow our plants!</t>
+  </si>
+  <si>
+    <t>Looks like we landed in a peculiar place where the weather is a little bit cooler than usual.</t>
+  </si>
+  <si>
+    <t>This is known as a microclimate, where the local atmospheric condition can differ from the surrounding areas.</t>
+  </si>
+  <si>
+    <t>Uh oh, a mushroom started to grow near our plants!</t>
+  </si>
+  <si>
+    <t>Their spores appear to be harmful to all our frogs and plants, but one: the iron frog!</t>
+  </si>
+  <si>
+    <t>Just as the iron frogs can rid us of the moles, they, too, can rid us of these mushrooms.</t>
+  </si>
+  <si>
+    <t>Since there’s a lot of moisture in the region, the fungi that grow these mushrooms from beneath are able to absorb a lot of nutrients.</t>
+  </si>
+  <si>
+    <t>In our case, we are below the slope of a hill that obscures most of the sunlight, and precipitations linger around longer.</t>
   </si>
 </sst>
 </file>
@@ -1819,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D172"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,623 +2235,623 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>485</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="B51" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>286</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>287</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B54" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>247</v>
+        <v>293</v>
       </c>
       <c r="B57" t="s">
-        <v>248</v>
-      </c>
-      <c r="C57">
-        <v>1.5</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>247</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>248</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C59">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>184</v>
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>251</v>
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>16</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="C65">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>185</v>
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>22</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>252</v>
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>73</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" t="s">
-        <v>83</v>
+        <v>72</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>253</v>
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>83</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>254</v>
+        <v>86</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>89</v>
+        <v>254</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>186</v>
+        <v>89</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>255</v>
+        <v>93</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>255</v>
       </c>
       <c r="C77">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>256</v>
+        <v>97</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>104</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>257</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>105</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C83">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>259</v>
+        <v>108</v>
       </c>
       <c r="C84">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>259</v>
       </c>
       <c r="C85">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>260</v>
+        <v>165</v>
+      </c>
+      <c r="B86" t="s">
+        <v>167</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>29</v>
-      </c>
-      <c r="B87" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="C87">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>168</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>244</v>
       </c>
       <c r="C89">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>261</v>
+        <v>169</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>170</v>
+        <v>261</v>
       </c>
       <c r="C91">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>32</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>262</v>
+        <v>31</v>
+      </c>
+      <c r="B92" t="s">
+        <v>170</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" t="s">
-        <v>173</v>
+        <v>32</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="C93">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>172</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>263</v>
+        <v>171</v>
+      </c>
+      <c r="B94" t="s">
+        <v>173</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>174</v>
-      </c>
-      <c r="B95" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="C95">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>176</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>264</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
         <v>42</v>
@@ -2778,15 +2859,15 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" t="s">
         <v>46</v>
@@ -2794,15 +2875,15 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B101" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B102" t="s">
         <v>49</v>
@@ -2810,688 +2891,792 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B103" t="s">
-        <v>160</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B104" t="s">
-        <v>282</v>
+        <v>160</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>282</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>265</v>
+        <v>52</v>
+      </c>
+      <c r="B106" t="s">
+        <v>53</v>
       </c>
       <c r="C106">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>55</v>
-      </c>
-      <c r="B107" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>56</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>266</v>
+        <v>55</v>
+      </c>
+      <c r="B108" t="s">
+        <v>138</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>57</v>
-      </c>
-      <c r="B109" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>266</v>
       </c>
       <c r="C109">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>267</v>
+        <v>58</v>
       </c>
       <c r="C110">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B112" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C112">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B114" t="s">
-        <v>268</v>
+        <v>63</v>
       </c>
       <c r="C114">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>191</v>
+        <v>268</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>269</v>
+        <v>191</v>
       </c>
       <c r="C116">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B117" t="s">
-        <v>65</v>
+        <v>269</v>
       </c>
       <c r="C117">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>272</v>
+        <v>65</v>
       </c>
       <c r="C118">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="B119" t="s">
-        <v>68</v>
+        <v>272</v>
       </c>
       <c r="C119">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>192</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>270</v>
+        <v>67</v>
+      </c>
+      <c r="B120" t="s">
+        <v>68</v>
       </c>
       <c r="C120">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>90</v>
-      </c>
-      <c r="B121" t="s">
-        <v>91</v>
+        <v>192</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="C121">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B122" t="s">
-        <v>273</v>
+        <v>91</v>
       </c>
       <c r="C122">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>80</v>
+        <v>273</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>195</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>271</v>
+        <v>79</v>
+      </c>
+      <c r="B124" t="s">
+        <v>80</v>
       </c>
       <c r="C124">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>198</v>
+        <v>271</v>
       </c>
       <c r="C125">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>274</v>
+        <v>198</v>
       </c>
       <c r="C126">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>98</v>
-      </c>
-      <c r="B127" t="s">
-        <v>99</v>
+        <v>197</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>199</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>278</v>
+        <v>98</v>
+      </c>
+      <c r="B128" t="s">
+        <v>99</v>
       </c>
       <c r="C128">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>202</v>
+        <v>278</v>
       </c>
       <c r="C129">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>277</v>
+        <v>202</v>
       </c>
       <c r="C130">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>203</v>
+        <v>277</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>276</v>
+        <v>203</v>
       </c>
       <c r="C132">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>208</v>
+        <v>276</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>275</v>
+        <v>208</v>
       </c>
       <c r="C134">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>177</v>
-      </c>
-      <c r="B135" t="s">
-        <v>279</v>
+        <v>207</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C135">
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B136" t="s">
-        <v>181</v>
+        <v>279</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B137" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="B139" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>74</v>
       </c>
       <c r="B140" t="s">
-        <v>246</v>
-      </c>
-      <c r="C140">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="B141" t="s">
-        <v>213</v>
+        <v>246</v>
       </c>
       <c r="C141">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>214</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>291</v>
+        <v>212</v>
+      </c>
+      <c r="B142" t="s">
+        <v>213</v>
       </c>
       <c r="C142">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C143">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>216</v>
-      </c>
-      <c r="B144" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C144">
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B145" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B146" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B147" t="s">
-        <v>227</v>
-      </c>
-      <c r="C147">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>228</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>280</v>
+        <v>226</v>
+      </c>
+      <c r="B148" t="s">
+        <v>227</v>
       </c>
       <c r="C148">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>229</v>
-      </c>
-      <c r="B149" t="s">
-        <v>231</v>
+        <v>228</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B150" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="C150">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B151" t="s">
-        <v>234</v>
+        <v>281</v>
+      </c>
+      <c r="C151">
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B152" t="s">
-        <v>446</v>
+        <v>234</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B153" t="s">
-        <v>236</v>
-      </c>
-      <c r="C153">
-        <v>3</v>
+        <v>446</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B154" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B155" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>450</v>
+        <v>235</v>
       </c>
       <c r="B156" t="s">
-        <v>478</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B157" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B158" t="s">
-        <v>454</v>
+        <v>478</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B159" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B160" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B161" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B162" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B163" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B164" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B165" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B166" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B167" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B168" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B169" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>472</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>477</v>
+        <v>471</v>
+      </c>
+      <c r="B170" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>473</v>
-      </c>
-      <c r="B171" t="s">
-        <v>475</v>
+        <v>472</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>473</v>
+      </c>
+      <c r="B172" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>474</v>
       </c>
-      <c r="B172" t="s">
-        <v>476</v>
+      <c r="B173" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>483</v>
+      </c>
+      <c r="B174" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>489</v>
+      </c>
+      <c r="B175" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>490</v>
+      </c>
+      <c r="B176" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>491</v>
+      </c>
+      <c r="B177" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>492</v>
+      </c>
+      <c r="B178" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>493</v>
+      </c>
+      <c r="B179" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>494</v>
+      </c>
+      <c r="B180" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>495</v>
+      </c>
+      <c r="B181" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>496</v>
+      </c>
+      <c r="B182" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>497</v>
+      </c>
+      <c r="B183" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>498</v>
+      </c>
+      <c r="B184" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>499</v>
+      </c>
+      <c r="B185" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -3502,10 +3687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D172"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3837,623 +4022,623 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>485</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>326</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>283</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="B51" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B52" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>286</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>247</v>
+        <v>293</v>
       </c>
       <c r="B57" t="s">
-        <v>346</v>
-      </c>
-      <c r="C57">
-        <v>1.5</v>
+        <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>247</v>
       </c>
       <c r="B58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C59">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>349</v>
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>348</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" t="s">
-        <v>350</v>
+        <v>13</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>351</v>
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>350</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" t="s">
-        <v>352</v>
+        <v>18</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>353</v>
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>352</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" t="s">
-        <v>354</v>
+        <v>15</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="C65">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>355</v>
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>354</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" t="s">
-        <v>356</v>
+        <v>21</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>357</v>
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>356</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" t="s">
-        <v>358</v>
+        <v>72</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>359</v>
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>358</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" t="s">
-        <v>354</v>
+        <v>82</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>359</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C77">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C83">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C84">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C85">
-        <v>1.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>374</v>
+        <v>165</v>
+      </c>
+      <c r="B86" t="s">
+        <v>373</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>29</v>
-      </c>
-      <c r="B87" t="s">
-        <v>375</v>
+        <v>166</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>374</v>
       </c>
       <c r="C87">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C89">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B91" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C91">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>32</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>380</v>
+        <v>31</v>
+      </c>
+      <c r="B92" t="s">
+        <v>379</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" t="s">
-        <v>381</v>
+        <v>32</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>380</v>
       </c>
       <c r="C93">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>172</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>382</v>
+        <v>171</v>
+      </c>
+      <c r="B94" t="s">
+        <v>381</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>174</v>
-      </c>
-      <c r="B95" t="s">
-        <v>383</v>
+        <v>172</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>382</v>
       </c>
       <c r="C95">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>384</v>
+      </c>
+      <c r="C97">
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
         <v>42</v>
@@ -4461,15 +4646,15 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B99" t="s">
-        <v>334</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" t="s">
         <v>334</v>
@@ -4477,15 +4662,15 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B101" t="s">
-        <v>49</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B102" t="s">
         <v>49</v>
@@ -4493,637 +4678,705 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B103" t="s">
-        <v>385</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B104" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>386</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>387</v>
+        <v>52</v>
+      </c>
+      <c r="B106" t="s">
+        <v>53</v>
       </c>
       <c r="C106">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>55</v>
-      </c>
-      <c r="B107" t="s">
-        <v>388</v>
+        <v>54</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>387</v>
       </c>
       <c r="C107">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>56</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>389</v>
+        <v>55</v>
+      </c>
+      <c r="B108" t="s">
+        <v>388</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>57</v>
-      </c>
-      <c r="B109" t="s">
-        <v>390</v>
+        <v>56</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C109">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C110">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B112" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C112">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B114" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C114">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C116">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B117" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C117">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C118">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
       <c r="B119" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C119">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>192</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>401</v>
+        <v>67</v>
+      </c>
+      <c r="B120" t="s">
+        <v>400</v>
       </c>
       <c r="C120">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>90</v>
-      </c>
-      <c r="B121" t="s">
-        <v>402</v>
+        <v>192</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C121">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="B122" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C122">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>195</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>405</v>
+        <v>79</v>
+      </c>
+      <c r="B124" t="s">
+        <v>404</v>
       </c>
       <c r="C124">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>198</v>
+        <v>405</v>
       </c>
       <c r="C125">
-        <v>2.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>406</v>
+        <v>198</v>
       </c>
       <c r="C126">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>98</v>
-      </c>
-      <c r="B127" t="s">
-        <v>407</v>
+        <v>197</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>406</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>199</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>408</v>
+        <v>98</v>
+      </c>
+      <c r="B128" t="s">
+        <v>407</v>
       </c>
       <c r="C128">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>202</v>
+        <v>408</v>
       </c>
       <c r="C129">
-        <v>1.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>409</v>
+        <v>202</v>
       </c>
       <c r="C130">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C132">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>208</v>
+        <v>411</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>412</v>
+        <v>208</v>
       </c>
       <c r="C134">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>177</v>
-      </c>
-      <c r="B135" t="s">
-        <v>413</v>
+        <v>207</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C135">
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B136" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="B137" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="B139" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>245</v>
+        <v>74</v>
       </c>
       <c r="B140" t="s">
-        <v>418</v>
-      </c>
-      <c r="C140">
-        <v>8</v>
+        <v>417</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="B141" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C141">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>214</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>420</v>
+        <v>212</v>
+      </c>
+      <c r="B142" t="s">
+        <v>419</v>
       </c>
       <c r="C142">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C143">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>216</v>
-      </c>
-      <c r="B144" t="s">
-        <v>422</v>
+        <v>215</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C144">
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B145" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B146" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B147" t="s">
-        <v>425</v>
-      </c>
-      <c r="C147">
-        <v>2</v>
+        <v>424</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>228</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>426</v>
+        <v>226</v>
+      </c>
+      <c r="B148" t="s">
+        <v>425</v>
       </c>
       <c r="C148">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>229</v>
-      </c>
-      <c r="B149" t="s">
-        <v>427</v>
+        <v>228</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>426</v>
       </c>
       <c r="C149">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B150" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C150">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B151" t="s">
-        <v>429</v>
+        <v>428</v>
+      </c>
+      <c r="C151">
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B152" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B153" t="s">
-        <v>430</v>
-      </c>
-      <c r="C153">
-        <v>3</v>
+        <v>445</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B154" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B155" t="s">
-        <v>432</v>
+        <v>431</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>450</v>
+        <v>235</v>
+      </c>
+      <c r="B156" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>474</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
level 3 intro dialog stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38126D0-1DEE-4445-B985-5DB131DED054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89226E1F-F4B0-45ED-8ABC-695FCFDC959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="2355" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5970" yWindow="2115" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="539">
   <si>
     <t>Key</t>
   </si>
@@ -1535,15 +1535,9 @@
     <t>Nevertheless, this moody atmosphere is a perfect place to grow our plants!</t>
   </si>
   <si>
-    <t>Looks like we landed in a peculiar place where the weather is a little bit cooler than usual.</t>
-  </si>
-  <si>
     <t>This is known as a microclimate, where the local atmospheric condition can differ from the surrounding areas.</t>
   </si>
   <si>
-    <t>Uh oh, a mushroom started to grow near our plants!</t>
-  </si>
-  <si>
     <t>Their spores appear to be harmful to all our frogs and plants, but one: the iron frog!</t>
   </si>
   <si>
@@ -1554,6 +1548,96 @@
   </si>
   <si>
     <t>In our case, we are below the slope of a hill that obscures most of the sunlight, and precipitations linger around longer.</t>
+  </si>
+  <si>
+    <t>intro_climate_desert_01</t>
+  </si>
+  <si>
+    <t>Uh oh, a mushroom started to grow near one of our plants!</t>
+  </si>
+  <si>
+    <t>Looks like we landed in a peculiar place where the weather is a little bit colder than usual.</t>
+  </si>
+  <si>
+    <t>intro_climate_desert_02</t>
+  </si>
+  <si>
+    <t>intro_climate_desert_03</t>
+  </si>
+  <si>
+    <t>Oh boy, the desert climate...We sure took a wrong turn when we landed.</t>
+  </si>
+  <si>
+    <t>This dry and hot weather will leave us with little to no water for our plants…and with dry soil, not much nutrients are available.</t>
+  </si>
+  <si>
+    <t>However, there are oases nearby! This miracle of a microclimate will allow us to gather nutrients and water for our plants!</t>
+  </si>
+  <si>
+    <t>hopper_intro_01</t>
+  </si>
+  <si>
+    <t>hopper_intro_02</t>
+  </si>
+  <si>
+    <t>hopper_intro_03</t>
+  </si>
+  <si>
+    <t>hopper_intro_04</t>
+  </si>
+  <si>
+    <t>Watch out, it's a grasshopper!</t>
+  </si>
+  <si>
+    <t>These hopping hooligans can strive even in the hottest of climates, and they're no picky eaters either!</t>
+  </si>
+  <si>
+    <t>antlion_intro_01</t>
+  </si>
+  <si>
+    <t>antlion_intro_02</t>
+  </si>
+  <si>
+    <t>antlion_intro_03</t>
+  </si>
+  <si>
+    <t>antlion_intro_04</t>
+  </si>
+  <si>
+    <t>An antlion larva has been spotted!</t>
+  </si>
+  <si>
+    <t>These insects are commonly found in dry and sandy climates where they can easily excavate their pits.</t>
+  </si>
+  <si>
+    <t>Our poor unsuspecting frogs will fall prey to these pits if left alone.</t>
+  </si>
+  <si>
+    <t>Deploy the iron frog to plug away these troublesome pits for good!</t>
+  </si>
+  <si>
+    <t>hazard_weather_intro_01</t>
+  </si>
+  <si>
+    <t>hazard_weather_intro_02</t>
+  </si>
+  <si>
+    <t>hazard_weather_intro_03</t>
+  </si>
+  <si>
+    <t>Take cover, for there is a sand storm heading our way!</t>
+  </si>
+  <si>
+    <t>Every once in a while, in certain regions, a dangerous atmospheric condition occurs that can cause major destruction.</t>
+  </si>
+  <si>
+    <t>Make sure to deploy any of these frogs to stop them on their tracks!</t>
+  </si>
+  <si>
+    <t>These ones in particular have powerful hind legs that emit a dangerous wave that harms our frogs!</t>
+  </si>
+  <si>
+    <t>With proper equipment and knowledge of weather pattern, one can properly prepare, and even avoid these severe weathers.</t>
   </si>
 </sst>
 </file>
@@ -1900,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,7 +3712,7 @@
         <v>493</v>
       </c>
       <c r="B179" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3636,7 +3720,7 @@
         <v>494</v>
       </c>
       <c r="B180" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3644,7 +3728,7 @@
         <v>495</v>
       </c>
       <c r="B181" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3652,7 +3736,7 @@
         <v>496</v>
       </c>
       <c r="B182" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3660,7 +3744,7 @@
         <v>497</v>
       </c>
       <c r="B183" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3668,7 +3752,7 @@
         <v>498</v>
       </c>
       <c r="B184" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3676,7 +3760,119 @@
         <v>499</v>
       </c>
       <c r="B185" t="s">
-        <v>508</v>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>509</v>
+      </c>
+      <c r="B186" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>512</v>
+      </c>
+      <c r="B187" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>513</v>
+      </c>
+      <c r="B188" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>517</v>
+      </c>
+      <c r="B189" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>518</v>
+      </c>
+      <c r="B190" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>519</v>
+      </c>
+      <c r="B191" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>520</v>
+      </c>
+      <c r="B192" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>523</v>
+      </c>
+      <c r="B193" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>524</v>
+      </c>
+      <c r="B194" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>525</v>
+      </c>
+      <c r="B195" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>526</v>
+      </c>
+      <c r="B196" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>531</v>
+      </c>
+      <c r="B197" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>532</v>
+      </c>
+      <c r="B198" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>533</v>
+      </c>
+      <c r="B199" t="s">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -3687,10 +3883,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D199"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200:XFD200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5379,6 +5575,76 @@
         <v>499</v>
       </c>
     </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>533</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
level 4 intro dialog
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89226E1F-F4B0-45ED-8ABC-695FCFDC959F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6404D94-E48F-4252-BD63-2E1FD05B91A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="2115" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="551">
   <si>
     <t>Key</t>
   </si>
@@ -1638,6 +1638,42 @@
   </si>
   <si>
     <t>With proper equipment and knowledge of weather pattern, one can properly prepare, and even avoid these severe weathers.</t>
+  </si>
+  <si>
+    <t>coldAnnually</t>
+  </si>
+  <si>
+    <t>Cold and freezing all year round.</t>
+  </si>
+  <si>
+    <t>intro_climate_polar_01</t>
+  </si>
+  <si>
+    <t>intro_climate_polar_02</t>
+  </si>
+  <si>
+    <t>intro_climate_polar_03</t>
+  </si>
+  <si>
+    <t>intro_climate_polar_04</t>
+  </si>
+  <si>
+    <t>intro_climate_polar_05</t>
+  </si>
+  <si>
+    <t>Brrrtz! This climate is as cold as it can get!</t>
+  </si>
+  <si>
+    <t>Only the sturdiest of plants can withstand this bitter cold. Luckily for us, we happen to have the right tools to allow our plants to grow.</t>
+  </si>
+  <si>
+    <t>Now go forth, and grow the last batch of our plants!</t>
+  </si>
+  <si>
+    <t>Most of the regions under the polar climate are far away from the equator.</t>
+  </si>
+  <si>
+    <t>Hence, the weather patterns consisting of cool summers and very cold winters.</t>
   </si>
 </sst>
 </file>
@@ -1984,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B199" sqref="B199"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="B204" sqref="B204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3875,6 +3911,54 @@
         <v>538</v>
       </c>
     </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>539</v>
+      </c>
+      <c r="B200" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>541</v>
+      </c>
+      <c r="B201" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>542</v>
+      </c>
+      <c r="B202" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>543</v>
+      </c>
+      <c r="B203" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>544</v>
+      </c>
+      <c r="B204" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>545</v>
+      </c>
+      <c r="B205" t="s">
+        <v>548</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3883,10 +3967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:XFD200"/>
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5645,6 +5729,36 @@
         <v>533</v>
       </c>
     </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
some unit tweaks, complete the game automatically, allow players to fill all climate matches in post game completely.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6404D94-E48F-4252-BD63-2E1FD05B91A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D66769-C897-4CC6-A0BE-811F2E0C5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="553">
   <si>
     <t>Key</t>
   </si>
@@ -1674,6 +1674,12 @@
   </si>
   <si>
     <t>Hence, the weather patterns consisting of cool summers and very cold winters.</t>
+  </si>
+  <si>
+    <t>dragClimateZone_instruction</t>
+  </si>
+  <si>
+    <t>Drag the climate types to the matching climate zones.</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204"/>
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3959,6 +3965,14 @@
         <v>548</v>
       </c>
     </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>551</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3967,10 +3981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+      <selection activeCell="A206" sqref="A206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5759,6 +5773,11 @@
         <v>545</v>
       </c>
     </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>551</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
some text adjustments, don't save config settings
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D66769-C897-4CC6-A0BE-811F2E0C5F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EE8856-F3C0-4D48-9830-E7763D76DCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1541,12 +1541,6 @@
     <t>Their spores appear to be harmful to all our frogs and plants, but one: the iron frog!</t>
   </si>
   <si>
-    <t>Just as the iron frogs can rid us of the moles, they, too, can rid us of these mushrooms.</t>
-  </si>
-  <si>
-    <t>Since there’s a lot of moisture in the region, the fungi that grow these mushrooms from beneath are able to absorb a lot of nutrients.</t>
-  </si>
-  <si>
     <t>In our case, we are below the slope of a hill that obscures most of the sunlight, and precipitations linger around longer.</t>
   </si>
   <si>
@@ -1631,15 +1625,9 @@
     <t>Every once in a while, in certain regions, a dangerous atmospheric condition occurs that can cause major destruction.</t>
   </si>
   <si>
-    <t>Make sure to deploy any of these frogs to stop them on their tracks!</t>
-  </si>
-  <si>
     <t>These ones in particular have powerful hind legs that emit a dangerous wave that harms our frogs!</t>
   </si>
   <si>
-    <t>With proper equipment and knowledge of weather pattern, one can properly prepare, and even avoid these severe weathers.</t>
-  </si>
-  <si>
     <t>coldAnnually</t>
   </si>
   <si>
@@ -1680,6 +1668,18 @@
   </si>
   <si>
     <t>Drag the climate types to the matching climate zones.</t>
+  </si>
+  <si>
+    <t>Since there's a lot of moisture in the region, the fungi that grow these mushrooms are able to absorb a lot of nutrients.</t>
+  </si>
+  <si>
+    <t>Deploy the iron frogs to rid us of these mushrooms.</t>
+  </si>
+  <si>
+    <t>Make sure to deploy any of these frogs to stop them in their tracks!</t>
+  </si>
+  <si>
+    <t>With proper equipment and knowledge of the weather pattern, one can properly prepare, and even avoid these severe weathers.</t>
   </si>
 </sst>
 </file>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,7 +3754,7 @@
         <v>493</v>
       </c>
       <c r="B179" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3770,7 +3770,7 @@
         <v>495</v>
       </c>
       <c r="B181" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3778,7 +3778,7 @@
         <v>496</v>
       </c>
       <c r="B182" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3786,7 +3786,7 @@
         <v>497</v>
       </c>
       <c r="B183" t="s">
-        <v>507</v>
+        <v>549</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3802,175 +3802,175 @@
         <v>499</v>
       </c>
       <c r="B185" t="s">
-        <v>506</v>
+        <v>550</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B186" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B187" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B188" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B189" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B190" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B191" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B192" t="s">
-        <v>536</v>
+        <v>551</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B193" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B194" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B195" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B196" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B197" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B198" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B199" t="s">
-        <v>538</v>
+        <v>552</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B200" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B201" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B202" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B203" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B204" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B205" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -5675,107 +5675,107 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shorten all cycle duration to 50 sec., more tweaks to levels, adjusted gardener AI, some language tweak
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EE8856-F3C0-4D48-9830-E7763D76DCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B28681-0D6C-4AF0-A7C9-73124DA0DEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="551">
   <si>
     <t>Key</t>
   </si>
@@ -1634,9 +1634,6 @@
     <t>Cold and freezing all year round.</t>
   </si>
   <si>
-    <t>intro_climate_polar_01</t>
-  </si>
-  <si>
     <t>intro_climate_polar_02</t>
   </si>
   <si>
@@ -1647,9 +1644,6 @@
   </si>
   <si>
     <t>intro_climate_polar_05</t>
-  </si>
-  <si>
-    <t>Brrrtz! This climate is as cold as it can get!</t>
   </si>
   <si>
     <t>Only the sturdiest of plants can withstand this bitter cold. Luckily for us, we happen to have the right tools to allow our plants to grow.</t>
@@ -2026,9 +2020,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+    <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
@@ -3031,7 +3025,7 @@
         <v>160</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3053,7 +3047,7 @@
         <v>53</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3075,7 +3069,7 @@
         <v>138</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3097,7 +3091,7 @@
         <v>58</v>
       </c>
       <c r="C110">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3119,7 +3113,7 @@
         <v>187</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3141,7 +3135,7 @@
         <v>63</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,7 +3780,7 @@
         <v>497</v>
       </c>
       <c r="B183" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3802,7 +3796,7 @@
         <v>499</v>
       </c>
       <c r="B185" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3858,7 +3852,7 @@
         <v>518</v>
       </c>
       <c r="B192" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3914,7 +3908,7 @@
         <v>531</v>
       </c>
       <c r="B199" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3930,7 +3924,7 @@
         <v>537</v>
       </c>
       <c r="B201" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3938,7 +3932,7 @@
         <v>538</v>
       </c>
       <c r="B202" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3946,7 +3940,7 @@
         <v>539</v>
       </c>
       <c r="B203" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3954,23 +3948,15 @@
         <v>540</v>
       </c>
       <c r="B204" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>541</v>
-      </c>
-      <c r="B205" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>547</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -3981,10 +3967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A206" sqref="A206"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4986,7 +4972,7 @@
         <v>385</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -5008,7 +4994,7 @@
         <v>53</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -5030,7 +5016,7 @@
         <v>388</v>
       </c>
       <c r="C108">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -5052,7 +5038,7 @@
         <v>390</v>
       </c>
       <c r="C110">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -5074,7 +5060,7 @@
         <v>392</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -5096,7 +5082,7 @@
         <v>394</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -5770,12 +5756,7 @@
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduced to one cycle for level 3 and 4. Moved severe weather explanation to level 4, removed severe weather in level 3. Made explanations to be child-proof.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B28681-0D6C-4AF0-A7C9-73124DA0DEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E44BD-A484-494D-BBA5-BEB9563C5987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9525" yWindow="1650" windowWidth="28365" windowHeight="18045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="1665" windowWidth="28365" windowHeight="18045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="529">
   <si>
     <t>Key</t>
   </si>
@@ -701,24 +701,6 @@
     <t>summer</t>
   </si>
   <si>
-    <t>level2Summary01</t>
-  </si>
-  <si>
-    <t>Microclimate</t>
-  </si>
-  <si>
-    <t>level2Summary02</t>
-  </si>
-  <si>
-    <t>level3Summary01</t>
-  </si>
-  <si>
-    <t>level3Summary02</t>
-  </si>
-  <si>
-    <t>Severe Weather</t>
-  </si>
-  <si>
     <t>postGameDialog01</t>
   </si>
   <si>
@@ -800,24 +782,6 @@
     <t>A moderate amount of snow accumulates over the day. Low visibility is expected.</t>
   </si>
   <si>
-    <t>A combination of strong wind, and freezing temperature. Falling large debris of ice is to be expected throughout the day.</t>
-  </si>
-  <si>
-    <t>These frogs will be gathering water from a nearby source. Please protect them as they traverse the land!</t>
-  </si>
-  <si>
-    <t>Deploy these hardy frogs to crush pesky rodents from the ground.</t>
-  </si>
-  <si>
-    <t>Deploy these frogs to fight against the pests that plague the sky.</t>
-  </si>
-  <si>
-    <t>These flies are capable of generating warmth to help flowers grow in cold weather, as well as melt ice.</t>
-  </si>
-  <si>
-    <t>Deploy these frogs to protect the flowers from being blown away by dangerous wind.</t>
-  </si>
-  <si>
     <t>Continental climates are found in regions away from the sea. They generally have four seasons: spring, summer, autumn, and winter.</t>
   </si>
   <si>
@@ -863,12 +827,6 @@
     <t>Welcome to Project Bloom! We are conducting an experiment to grow some special flowers in various climates.</t>
   </si>
   <si>
-    <t>Certain local areas can have a different pattern of weather than the main climate. This can be as small as a garden patch, or even a cave. As an example: a mountain or a hill can block the sunlight for most of the time, causing a cooler region.</t>
-  </si>
-  <si>
-    <t>These are rare types of weather that can cause havoc across a region. Their atmospheric condition such as the wind and temperature are off the charts. Severe weathers are considered to be dangerous, and can put you in a perilous situation.</t>
-  </si>
-  <si>
     <t>These climates are dry areas that receive little to no rain over a stretch of time. Not much vegetations can grow in these areas.</t>
   </si>
   <si>
@@ -923,9 +881,6 @@
     <t>CRÉDITOS</t>
   </si>
   <si>
-    <t>&lt;b&gt;Escrito por:&lt;/b&gt; David Dionisio\r\n&lt;b&gt;Música de:&lt;/b&gt; Kevin Macleod\r\n&lt;b&gt;Fotos:&lt;/b&gt;\r\nSahara (Kent Larsson), Camino a las Islas (Trevor Wright), Río Similkameen (Greg Shine, BLM), Costa Brava (Gordito1869), Puerto Rico (Oquendo)</t>
-  </si>
-  <si>
     <t>LANZAMIENTO</t>
   </si>
   <si>
@@ -1157,27 +1112,15 @@
     <t>Rana de hierro</t>
   </si>
   <si>
-    <t>Despliega estas ranas resistentes para aplastar a molestos roedores del suelo.</t>
-  </si>
-  <si>
     <t>Rana de aire</t>
   </si>
   <si>
-    <t>Despliega estas ranas para luchar contra las plagas que azotan el cielo.</t>
-  </si>
-  <si>
     <t>Mosca Solar</t>
   </si>
   <si>
-    <t>Estas moscas son capaces de generar calor para ayudar a que las flores crezcan en climas fríos, así como derretir hielo.</t>
-  </si>
-  <si>
     <t>Rana del parabrisas</t>
   </si>
   <si>
-    <t>Despliega estas ranas para proteger las flores de la explosión del viento peligroso.</t>
-  </si>
-  <si>
     <t>Desierto</t>
   </si>
   <si>
@@ -1298,18 +1241,6 @@
     <t>Día 3</t>
   </si>
   <si>
-    <t>Microclima</t>
-  </si>
-  <si>
-    <t>Algunas zonas locales pueden tener un patrón de clima diferente al del clima principal. Esto puede ser tan pequeño como un parche de jardín o incluso una cueva. Por ejemplo: una montaña o una colina pueden bloquear la luz solar durante la mayor parte del tiempo, lo que provoca una región más fría.</t>
-  </si>
-  <si>
-    <t>Clima Severo</t>
-  </si>
-  <si>
-    <t>Estos son tipos raros de clima que pueden causar estragos en una región. Su estado atmosférico, como el viento y la temperatura, están fuera de las listas. Los climas severos se consideran peligrosos y pueden ponerlo en una situación peligrosa.</t>
-  </si>
-  <si>
     <t>Ahora que tenemos suficientes datos climáticos de la Tierra, solo tenemos que verificar su categoría en cada zona climática.</t>
   </si>
   <si>
@@ -1385,9 +1316,6 @@
     <t>intro_climate_continental_04</t>
   </si>
   <si>
-    <t>Without the ocean to moderate the temperature, not much can stop the prevailing wind from being too hot, or too cold.</t>
-  </si>
-  <si>
     <t>In this scenario, we will be growing our plants during summer. Where it is mostly sunny, with some rain here and there. A pleasant weather to be out and about, and grow our plants!</t>
   </si>
   <si>
@@ -1427,9 +1355,6 @@
     <t>Watch out! It looks like weeds are starting to grow near one of our plants!</t>
   </si>
   <si>
-    <t>Though the weather is ideal for our plants, unfortunately so it will be for these intrusive plants.</t>
-  </si>
-  <si>
     <t>mole_intro_01</t>
   </si>
   <si>
@@ -1457,15 +1382,9 @@
     <t>In continental climates, the temperature varies throughout the year.</t>
   </si>
   <si>
-    <t>This is due to the region being within large landmasses far away from the oceans.</t>
-  </si>
-  <si>
     <t>We must get rid of them, or else they will suck away all the nutrients that our plants need to grow!</t>
   </si>
   <si>
-    <t>A mole! These subterranean insectivores can be commonly found in continental climates, where the soil is ideal for making tunnels.</t>
-  </si>
-  <si>
     <t>While moles don't have much interest in veggies, their tunneling however, can ruin a plant's roots.</t>
   </si>
   <si>
@@ -1502,15 +1421,6 @@
     <t>intro_climate_oceanic_04</t>
   </si>
   <si>
-    <t>intro_microclimate_01</t>
-  </si>
-  <si>
-    <t>intro_microclimate_02</t>
-  </si>
-  <si>
-    <t>intro_microclimate_03</t>
-  </si>
-  <si>
     <t>mushroom_intro_01</t>
   </si>
   <si>
@@ -1526,33 +1436,18 @@
     <t>Ah, the oceanic climate! Where it’s nice and cool throughout the year!</t>
   </si>
   <si>
-    <t>This is due to the region being close to the ocean that regulates the temperature.</t>
-  </si>
-  <si>
     <t>However, the winds carrying the nice ocean breeze can cause a lot of days to be dull and dreary.</t>
   </si>
   <si>
     <t>Nevertheless, this moody atmosphere is a perfect place to grow our plants!</t>
   </si>
   <si>
-    <t>This is known as a microclimate, where the local atmospheric condition can differ from the surrounding areas.</t>
-  </si>
-  <si>
-    <t>Their spores appear to be harmful to all our frogs and plants, but one: the iron frog!</t>
-  </si>
-  <si>
-    <t>In our case, we are below the slope of a hill that obscures most of the sunlight, and precipitations linger around longer.</t>
-  </si>
-  <si>
     <t>intro_climate_desert_01</t>
   </si>
   <si>
     <t>Uh oh, a mushroom started to grow near one of our plants!</t>
   </si>
   <si>
-    <t>Looks like we landed in a peculiar place where the weather is a little bit colder than usual.</t>
-  </si>
-  <si>
     <t>intro_climate_desert_02</t>
   </si>
   <si>
@@ -1565,9 +1460,6 @@
     <t>This dry and hot weather will leave us with little to no water for our plants…and with dry soil, not much nutrients are available.</t>
   </si>
   <si>
-    <t>However, there are oases nearby! This miracle of a microclimate will allow us to gather nutrients and water for our plants!</t>
-  </si>
-  <si>
     <t>hopper_intro_01</t>
   </si>
   <si>
@@ -1583,9 +1475,6 @@
     <t>Watch out, it's a grasshopper!</t>
   </si>
   <si>
-    <t>These hopping hooligans can strive even in the hottest of climates, and they're no picky eaters either!</t>
-  </si>
-  <si>
     <t>antlion_intro_01</t>
   </si>
   <si>
@@ -1601,15 +1490,6 @@
     <t>An antlion larva has been spotted!</t>
   </si>
   <si>
-    <t>These insects are commonly found in dry and sandy climates where they can easily excavate their pits.</t>
-  </si>
-  <si>
-    <t>Our poor unsuspecting frogs will fall prey to these pits if left alone.</t>
-  </si>
-  <si>
-    <t>Deploy the iron frog to plug away these troublesome pits for good!</t>
-  </si>
-  <si>
     <t>hazard_weather_intro_01</t>
   </si>
   <si>
@@ -1619,15 +1499,9 @@
     <t>hazard_weather_intro_03</t>
   </si>
   <si>
-    <t>Take cover, for there is a sand storm heading our way!</t>
-  </si>
-  <si>
     <t>Every once in a while, in certain regions, a dangerous atmospheric condition occurs that can cause major destruction.</t>
   </si>
   <si>
-    <t>These ones in particular have powerful hind legs that emit a dangerous wave that harms our frogs!</t>
-  </si>
-  <si>
     <t>coldAnnually</t>
   </si>
   <si>
@@ -1670,10 +1544,70 @@
     <t>Deploy the iron frogs to rid us of these mushrooms.</t>
   </si>
   <si>
-    <t>Make sure to deploy any of these frogs to stop them in their tracks!</t>
-  </si>
-  <si>
     <t>With proper equipment and knowledge of the weather pattern, one can properly prepare, and even avoid these severe weathers.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Escrito por:&lt;/b&gt; David Dionisio\n&lt;b&gt;Música de:&lt;/b&gt; Kevin Macleod\n&lt;b&gt;Fotos:&lt;/b&gt;\nSahara (Kent Larsson), Camino a las Islas (Trevor Wright), Río Similkameen (Greg Shine, BLM), Costa Brava (Gordito1869), Puerto Rico (Oquendo)</t>
+  </si>
+  <si>
+    <t>Fortunately, there are oases nearby!</t>
+  </si>
+  <si>
+    <t>This is due to the region being within huge lands far away from the oceans.</t>
+  </si>
+  <si>
+    <t>Without the ocean to control the temperature, not much can stop the wind from being too hot, or too cold.</t>
+  </si>
+  <si>
+    <t>Though the weather is ideal for our plants, unfortunately so it will be for these invasive plants.</t>
+  </si>
+  <si>
+    <t>A mole! These underground insectivores can be commonly found in continental climates, where the soil is ideal for making tunnels.</t>
+  </si>
+  <si>
+    <t>This is due to the region being close to the ocean that controls the temperature.</t>
+  </si>
+  <si>
+    <t>Their spores appear to be harmful to all our frogs and plants, except the iron frog!</t>
+  </si>
+  <si>
+    <t>These hopping hooligans can survive even in the hottest of climates, and they're no picky eaters either!</t>
+  </si>
+  <si>
+    <t>These ones in particular have powerful legs that can cause harm to our frogs!</t>
+  </si>
+  <si>
+    <t>Have these frogs stop them in their tracks!</t>
+  </si>
+  <si>
+    <t>These insects are commonly found in dry and sandy climates where they can easily dig their pits.</t>
+  </si>
+  <si>
+    <t>Our poor defenseless frogs will fall prey to these pits if left alone.</t>
+  </si>
+  <si>
+    <t>Deploy the iron frog to plug away those troublesome pits for good!</t>
+  </si>
+  <si>
+    <t>A combination of strong wind, and freezing temperature. Falling large chunks of ice is to be expected throughout the day.</t>
+  </si>
+  <si>
+    <t>These frogs will be gathering water from a nearby oasis. Please protect them as they travel the land!</t>
+  </si>
+  <si>
+    <t>Place these hardy frogs towards the enemies to fight them off.</t>
+  </si>
+  <si>
+    <t>Place these frogs up in the sky to fight off flying pests.</t>
+  </si>
+  <si>
+    <t>These flies can generate warmth to help flowers grow in cold weather, as well as melt ice.</t>
+  </si>
+  <si>
+    <t>Place these frogs against the dangerous winds to protect the flowers from being blown away.</t>
+  </si>
+  <si>
+    <t>Take cover, a blizzard is heading our way!</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="B199" sqref="B199"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,15 +2009,15 @@
         <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,10 +2062,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="B11" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,26 +2118,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="B18" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B19" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -2225,7 +2159,7 @@
         <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -2247,7 +2181,7 @@
         <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -2323,10 +2257,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="B32" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2347,18 +2281,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="B35" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B36" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,10 +2409,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,42 +2433,42 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B54" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B55" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B56" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B57" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -2611,7 +2545,7 @@
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C65">
         <v>5</v>
@@ -2655,7 +2589,7 @@
         <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C69">
         <v>5</v>
@@ -2677,7 +2611,7 @@
         <v>82</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -2699,7 +2633,7 @@
         <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -2743,7 +2677,7 @@
         <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -2765,7 +2699,7 @@
         <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -2787,7 +2721,7 @@
         <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -2809,7 +2743,7 @@
         <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -2831,7 +2765,7 @@
         <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>259</v>
+        <v>522</v>
       </c>
       <c r="C85">
         <v>10</v>
@@ -2853,7 +2787,7 @@
         <v>166</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>260</v>
+        <v>523</v>
       </c>
       <c r="C87">
         <v>5</v>
@@ -2875,7 +2809,7 @@
         <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C89">
         <v>5</v>
@@ -2896,8 +2830,8 @@
       <c r="A91" t="s">
         <v>28</v>
       </c>
-      <c r="B91" t="s">
-        <v>261</v>
+      <c r="B91" s="4" t="s">
+        <v>524</v>
       </c>
       <c r="C91">
         <v>5</v>
@@ -2919,7 +2853,7 @@
         <v>32</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>262</v>
+        <v>525</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -2941,7 +2875,7 @@
         <v>172</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>263</v>
+        <v>526</v>
       </c>
       <c r="C95">
         <v>5</v>
@@ -2963,7 +2897,7 @@
         <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>264</v>
+        <v>527</v>
       </c>
       <c r="C97">
         <v>5</v>
@@ -3033,7 +2967,7 @@
         <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C105">
         <v>5</v>
@@ -3055,7 +2989,7 @@
         <v>54</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="C107">
         <v>8</v>
@@ -3077,7 +3011,7 @@
         <v>56</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C109">
         <v>8</v>
@@ -3099,7 +3033,7 @@
         <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="C111">
         <v>8</v>
@@ -3143,7 +3077,7 @@
         <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C115">
         <v>8</v>
@@ -3165,7 +3099,7 @@
         <v>190</v>
       </c>
       <c r="B117" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C117">
         <v>10</v>
@@ -3187,7 +3121,7 @@
         <v>193</v>
       </c>
       <c r="B119" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C119">
         <v>10</v>
@@ -3209,7 +3143,7 @@
         <v>192</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C121">
         <v>10</v>
@@ -3231,7 +3165,7 @@
         <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C123">
         <v>12</v>
@@ -3253,7 +3187,7 @@
         <v>195</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C125">
         <v>12</v>
@@ -3275,7 +3209,7 @@
         <v>197</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C127">
         <v>8</v>
@@ -3297,7 +3231,7 @@
         <v>199</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C129">
         <v>10</v>
@@ -3319,7 +3253,7 @@
         <v>201</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C131">
         <v>8</v>
@@ -3341,7 +3275,7 @@
         <v>205</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C133">
         <v>10</v>
@@ -3363,7 +3297,7 @@
         <v>207</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="C135">
         <v>10</v>
@@ -3374,7 +3308,7 @@
         <v>177</v>
       </c>
       <c r="B136" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3411,10 +3345,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B141" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C141">
         <v>8</v>
@@ -3436,7 +3370,7 @@
         <v>214</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="C143">
         <v>8</v>
@@ -3447,7 +3381,7 @@
         <v>215</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="C144">
         <v>10</v>
@@ -3482,481 +3416,413 @@
         <v>226</v>
       </c>
       <c r="B148" t="s">
-        <v>227</v>
-      </c>
-      <c r="C148">
-        <v>2</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>228</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C149">
-        <v>10</v>
+        <v>227</v>
+      </c>
+      <c r="B149" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B150" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B151" t="s">
-        <v>281</v>
+        <v>234</v>
       </c>
       <c r="C151">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B152" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>233</v>
+        <v>427</v>
       </c>
       <c r="B153" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>238</v>
+        <v>428</v>
       </c>
       <c r="B154" t="s">
-        <v>236</v>
-      </c>
-      <c r="C154">
-        <v>3</v>
+        <v>510</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>237</v>
+        <v>429</v>
       </c>
       <c r="B155" t="s">
-        <v>240</v>
-      </c>
-      <c r="C155">
-        <v>5</v>
+        <v>511</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>235</v>
+        <v>430</v>
       </c>
       <c r="B156" t="s">
-        <v>239</v>
+        <v>431</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="B157" t="s">
-        <v>477</v>
+        <v>436</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="B158" t="s">
-        <v>478</v>
+        <v>437</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="B159" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B160" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="B161" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="B162" t="s">
-        <v>461</v>
+        <v>512</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="B163" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>459</v>
-      </c>
-      <c r="B164" t="s">
-        <v>463</v>
+        <v>444</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="B165" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="B166" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>466</v>
-      </c>
-      <c r="B167" t="s">
-        <v>479</v>
+        <v>447</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="B168" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="B169" t="s">
-        <v>481</v>
+        <v>450</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="B170" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>472</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>476</v>
+        <v>462</v>
+      </c>
+      <c r="B171" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="B172" t="s">
-        <v>488</v>
+        <v>514</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="B173" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="B174" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="B175" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
       <c r="B176" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>491</v>
-      </c>
-      <c r="B177" t="s">
-        <v>502</v>
+        <v>468</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="B178" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="B179" t="s">
-        <v>509</v>
+        <v>477</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="B180" t="s">
-        <v>504</v>
+        <v>478</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>495</v>
-      </c>
-      <c r="B181" t="s">
-        <v>506</v>
+        <v>476</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="B182" t="s">
-        <v>508</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>497</v>
-      </c>
-      <c r="B183" t="s">
-        <v>547</v>
+        <v>480</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>498</v>
-      </c>
-      <c r="B184" t="s">
-        <v>505</v>
+        <v>481</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>499</v>
-      </c>
-      <c r="B185" t="s">
-        <v>548</v>
+        <v>482</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="B186" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>510</v>
-      </c>
-      <c r="B187" t="s">
-        <v>513</v>
+        <v>485</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>511</v>
-      </c>
-      <c r="B188" t="s">
-        <v>514</v>
+        <v>486</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
       <c r="B189" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>516</v>
-      </c>
-      <c r="B190" t="s">
-        <v>520</v>
+        <v>489</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="B191" t="s">
-        <v>534</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="B192" t="s">
-        <v>549</v>
+        <v>507</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
       <c r="B193" t="s">
-        <v>525</v>
+        <v>494</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="B194" t="s">
-        <v>526</v>
+        <v>501</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
       <c r="B195" t="s">
-        <v>527</v>
+        <v>502</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="B196" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>529</v>
+        <v>498</v>
       </c>
       <c r="B197" t="s">
-        <v>532</v>
+        <v>500</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>530</v>
-      </c>
-      <c r="B198" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>531</v>
-      </c>
-      <c r="B199" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>535</v>
-      </c>
-      <c r="B200" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>537</v>
-      </c>
-      <c r="B201" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>538</v>
-      </c>
-      <c r="B202" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>539</v>
-      </c>
-      <c r="B203" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>540</v>
-      </c>
-      <c r="B204" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>545</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>546</v>
+        <v>503</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -3967,10 +3833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5742D5-F849-48AD-B210-72EE1666DB9E}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,7 +3866,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -4014,7 +3880,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4022,15 +3888,15 @@
         <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>300</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,7 +3904,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4046,7 +3912,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4054,7 +3920,7 @@
         <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,7 +3928,7 @@
         <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4070,15 +3936,15 @@
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="B11" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4086,7 +3952,7 @@
         <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4094,7 +3960,7 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4102,7 +3968,7 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,7 +3976,7 @@
         <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4118,7 +3984,7 @@
         <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4126,31 +3992,31 @@
         <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="B18" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B19" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -4161,7 +4027,7 @@
         <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C21">
         <v>1.5</v>
@@ -4172,7 +4038,7 @@
         <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -4183,7 +4049,7 @@
         <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -4194,7 +4060,7 @@
         <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -4205,7 +4071,7 @@
         <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -4216,7 +4082,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4224,7 +4090,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -4235,7 +4101,7 @@
         <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -4246,7 +4112,7 @@
         <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -4254,7 +4120,7 @@
         <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -4265,15 +4131,15 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="B32" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -4281,7 +4147,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -4289,23 +4155,23 @@
         <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="B35" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B36" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -4321,7 +4187,7 @@
         <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -4329,7 +4195,7 @@
         <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -4337,7 +4203,7 @@
         <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -4345,7 +4211,7 @@
         <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -4353,7 +4219,7 @@
         <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -4361,7 +4227,7 @@
         <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -4369,7 +4235,7 @@
         <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -4377,7 +4243,7 @@
         <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -4385,7 +4251,7 @@
         <v>155</v>
       </c>
       <c r="B46" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -4393,7 +4259,7 @@
         <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -4401,7 +4267,7 @@
         <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4409,7 +4275,7 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4417,15 +4283,15 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B51" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4433,7 +4299,7 @@
         <v>222</v>
       </c>
       <c r="B52" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,47 +4307,47 @@
         <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B54" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B55" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B56" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B57" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -4492,7 +4358,7 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -4503,7 +4369,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C60">
         <v>1.25</v>
@@ -4514,7 +4380,7 @@
         <v>13</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -4525,7 +4391,7 @@
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -4536,7 +4402,7 @@
         <v>18</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -4547,7 +4413,7 @@
         <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -4558,7 +4424,7 @@
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="C65">
         <v>5</v>
@@ -4569,7 +4435,7 @@
         <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C66">
         <v>1.25</v>
@@ -4580,7 +4446,7 @@
         <v>21</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -4591,7 +4457,7 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C68">
         <v>2</v>
@@ -4602,7 +4468,7 @@
         <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C69">
         <v>5</v>
@@ -4613,7 +4479,7 @@
         <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4624,7 +4490,7 @@
         <v>82</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C71">
         <v>5</v>
@@ -4635,7 +4501,7 @@
         <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4646,7 +4512,7 @@
         <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -4657,7 +4523,7 @@
         <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4668,7 +4534,7 @@
         <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C75">
         <v>5</v>
@@ -4679,7 +4545,7 @@
         <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4690,7 +4556,7 @@
         <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="C77">
         <v>5</v>
@@ -4701,7 +4567,7 @@
         <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="C78">
         <v>1.25</v>
@@ -4712,7 +4578,7 @@
         <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -4723,7 +4589,7 @@
         <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -4734,7 +4600,7 @@
         <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -4745,7 +4611,7 @@
         <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4756,7 +4622,7 @@
         <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -4767,7 +4633,7 @@
         <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="C84">
         <v>1.5</v>
@@ -4778,7 +4644,7 @@
         <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="C85">
         <v>10</v>
@@ -4789,7 +4655,7 @@
         <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="C86">
         <v>1.25</v>
@@ -4800,7 +4666,7 @@
         <v>166</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="C87">
         <v>5</v>
@@ -4811,7 +4677,7 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="C88">
         <v>1.25</v>
@@ -4822,7 +4688,7 @@
         <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="C89">
         <v>5</v>
@@ -4833,7 +4699,7 @@
         <v>27</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
       <c r="C90">
         <v>1.25</v>
@@ -4843,9 +4709,6 @@
       <c r="A91" t="s">
         <v>28</v>
       </c>
-      <c r="B91" t="s">
-        <v>378</v>
-      </c>
       <c r="C91">
         <v>5</v>
       </c>
@@ -4855,7 +4718,7 @@
         <v>31</v>
       </c>
       <c r="B92" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="C92">
         <v>1.25</v>
@@ -4865,9 +4728,7 @@
       <c r="A93" t="s">
         <v>32</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>380</v>
-      </c>
+      <c r="B93" s="4"/>
       <c r="C93">
         <v>5</v>
       </c>
@@ -4877,7 +4738,7 @@
         <v>171</v>
       </c>
       <c r="B94" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="C94">
         <v>1.25</v>
@@ -4887,9 +4748,7 @@
       <c r="A95" t="s">
         <v>172</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>382</v>
-      </c>
+      <c r="B95" s="4"/>
       <c r="C95">
         <v>5</v>
       </c>
@@ -4899,7 +4758,7 @@
         <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="C96">
         <v>1.5</v>
@@ -4909,9 +4768,6 @@
       <c r="A97" t="s">
         <v>175</v>
       </c>
-      <c r="B97" t="s">
-        <v>384</v>
-      </c>
       <c r="C97">
         <v>5</v>
       </c>
@@ -4937,7 +4793,7 @@
         <v>44</v>
       </c>
       <c r="B100" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -4945,7 +4801,7 @@
         <v>45</v>
       </c>
       <c r="B101" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4969,7 +4825,7 @@
         <v>50</v>
       </c>
       <c r="B104" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="C104">
         <v>1.5</v>
@@ -4980,7 +4836,7 @@
         <v>51</v>
       </c>
       <c r="B105" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="C105">
         <v>5</v>
@@ -5002,7 +4858,7 @@
         <v>54</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="C107">
         <v>8</v>
@@ -5013,7 +4869,7 @@
         <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="C108">
         <v>1.5</v>
@@ -5024,7 +4880,7 @@
         <v>56</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="C109">
         <v>8</v>
@@ -5035,7 +4891,7 @@
         <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -5046,7 +4902,7 @@
         <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="C111">
         <v>8</v>
@@ -5057,7 +4913,7 @@
         <v>60</v>
       </c>
       <c r="B112" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="C112">
         <v>1.5</v>
@@ -5068,7 +4924,7 @@
         <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="C113">
         <v>8</v>
@@ -5079,7 +4935,7 @@
         <v>62</v>
       </c>
       <c r="B114" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="C114">
         <v>1.5</v>
@@ -5090,7 +4946,7 @@
         <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="C115">
         <v>8</v>
@@ -5101,7 +4957,7 @@
         <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -5112,7 +4968,7 @@
         <v>190</v>
       </c>
       <c r="B117" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="C117">
         <v>10</v>
@@ -5123,7 +4979,7 @@
         <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="C118">
         <v>1.5</v>
@@ -5134,7 +4990,7 @@
         <v>193</v>
       </c>
       <c r="B119" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="C119">
         <v>10</v>
@@ -5145,7 +5001,7 @@
         <v>67</v>
       </c>
       <c r="B120" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="C120">
         <v>2.5</v>
@@ -5156,7 +5012,7 @@
         <v>192</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="C121">
         <v>10</v>
@@ -5167,7 +5023,7 @@
         <v>90</v>
       </c>
       <c r="B122" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="C122">
         <v>2.5</v>
@@ -5178,7 +5034,7 @@
         <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="C123">
         <v>12</v>
@@ -5189,7 +5045,7 @@
         <v>79</v>
       </c>
       <c r="B124" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="C124">
         <v>2</v>
@@ -5200,7 +5056,7 @@
         <v>195</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="C125">
         <v>12</v>
@@ -5222,7 +5078,7 @@
         <v>197</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="C127">
         <v>8</v>
@@ -5233,7 +5089,7 @@
         <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="C128">
         <v>2</v>
@@ -5244,7 +5100,7 @@
         <v>199</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="C129">
         <v>10</v>
@@ -5266,7 +5122,7 @@
         <v>201</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="C131">
         <v>8</v>
@@ -5277,7 +5133,7 @@
         <v>204</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -5288,7 +5144,7 @@
         <v>205</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="C133">
         <v>10</v>
@@ -5310,7 +5166,7 @@
         <v>207</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="C135">
         <v>10</v>
@@ -5321,7 +5177,7 @@
         <v>177</v>
       </c>
       <c r="B136" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -5329,7 +5185,7 @@
         <v>180</v>
       </c>
       <c r="B137" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -5337,7 +5193,7 @@
         <v>161</v>
       </c>
       <c r="B138" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,7 +5201,7 @@
         <v>162</v>
       </c>
       <c r="B139" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -5353,15 +5209,15 @@
         <v>74</v>
       </c>
       <c r="B140" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B141" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="C141">
         <v>8</v>
@@ -5372,7 +5228,7 @@
         <v>212</v>
       </c>
       <c r="B142" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="C142">
         <v>3</v>
@@ -5383,7 +5239,7 @@
         <v>214</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="C143">
         <v>8</v>
@@ -5394,7 +5250,7 @@
         <v>215</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
       <c r="C144">
         <v>10</v>
@@ -5405,7 +5261,7 @@
         <v>216</v>
       </c>
       <c r="B145" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5413,7 +5269,7 @@
         <v>218</v>
       </c>
       <c r="B146" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,7 +5277,7 @@
         <v>219</v>
       </c>
       <c r="B147" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5429,334 +5285,275 @@
         <v>226</v>
       </c>
       <c r="B148" t="s">
-        <v>425</v>
-      </c>
-      <c r="C148">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>228</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="C149">
-        <v>10</v>
+        <v>227</v>
+      </c>
+      <c r="B149" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B150" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B151" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="C151">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B152" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>233</v>
-      </c>
-      <c r="B153" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>238</v>
-      </c>
-      <c r="B154" t="s">
-        <v>430</v>
-      </c>
-      <c r="C154">
-        <v>3</v>
+        <v>428</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>237</v>
-      </c>
-      <c r="B155" t="s">
-        <v>431</v>
-      </c>
-      <c r="C155">
-        <v>5</v>
+        <v>429</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>235</v>
-      </c>
-      <c r="B156" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>510</v>
+        <v>485</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>511</v>
+        <v>486</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>529</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>545</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>